<commit_message>
Updating week 9 spreads
</commit_message>
<xml_diff>
--- a/PEAR/PEAR Football/y2025/Spreads/spreads_tracker_week9.xlsx
+++ b/PEAR/PEAR Football/y2025/Spreads/spreads_tracker_week9.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P52"/>
+  <dimension ref="A1:P54"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -516,40 +516,40 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Memphis</t>
+          <t>Washington State</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>South Florida</t>
+          <t>Toledo</t>
         </is>
       </c>
       <c r="D2" t="n">
-        <v>9.300000000000001</v>
+        <v>7</v>
       </c>
       <c r="E2" t="n">
-        <v>6.4</v>
+        <v>6.6</v>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>Memphis -3.0</t>
+          <t>Toledo -1.5</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>South Florida -3.5</t>
+          <t>Washington State -1.5</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>Memphis -2.9</t>
+          <t>Toledo -5.1</t>
         </is>
       </c>
       <c r="I2" t="n">
-        <v>2.9</v>
+        <v>-5.1</v>
       </c>
       <c r="J2" t="n">
-        <v>-3.5</v>
+        <v>1.5</v>
       </c>
       <c r="K2" t="inlineStr"/>
       <c r="L2" t="inlineStr"/>
@@ -566,40 +566,40 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Delaware</t>
+          <t>Memphis</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Middle Tennessee</t>
+          <t>South Florida</t>
         </is>
       </c>
       <c r="D3" t="n">
-        <v>3</v>
+        <v>9.300000000000001</v>
       </c>
       <c r="E3" t="n">
-        <v>5.9</v>
+        <v>6.4</v>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>Delaware -10.5</t>
+          <t>Memphis -3.0</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>Delaware -9.5</t>
+          <t>South Florida -3.5</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>Delaware -15.4</t>
+          <t>Memphis -2.9</t>
         </is>
       </c>
       <c r="I3" t="n">
-        <v>15.4</v>
+        <v>2.9</v>
       </c>
       <c r="J3" t="n">
-        <v>9.5</v>
+        <v>-3.5</v>
       </c>
       <c r="K3" t="inlineStr"/>
       <c r="L3" t="inlineStr"/>
@@ -616,37 +616,37 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Southern Miss</t>
+          <t>Delaware</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>UL Monroe</t>
+          <t>Middle Tennessee</t>
         </is>
       </c>
       <c r="D4" t="n">
-        <v>3.7</v>
+        <v>3</v>
       </c>
       <c r="E4" t="n">
-        <v>5.699999999999999</v>
+        <v>5.4</v>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>Southern Miss -10.0</t>
+          <t>Delaware -10.5</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>Southern Miss -10</t>
+          <t>Delaware -10</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>Southern Miss -15.7</t>
+          <t>Delaware -15.4</t>
         </is>
       </c>
       <c r="I4" t="n">
-        <v>15.7</v>
+        <v>15.4</v>
       </c>
       <c r="J4" t="n">
         <v>10</v>
@@ -678,7 +678,7 @@
         <v>3.1</v>
       </c>
       <c r="E5" t="n">
-        <v>5.5</v>
+        <v>5</v>
       </c>
       <c r="F5" t="inlineStr">
         <is>
@@ -687,7 +687,7 @@
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>Buffalo -10</t>
+          <t>Buffalo -10.5</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
@@ -699,7 +699,7 @@
         <v>15.5</v>
       </c>
       <c r="J5" t="n">
-        <v>10</v>
+        <v>10.5</v>
       </c>
       <c r="K5" t="inlineStr"/>
       <c r="L5" t="inlineStr"/>
@@ -816,40 +816,40 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Rice</t>
+          <t>Iowa State</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>UConn</t>
+          <t>BYU</t>
         </is>
       </c>
       <c r="D8" t="n">
-        <v>3.7</v>
+        <v>9.199999999999999</v>
       </c>
       <c r="E8" t="n">
-        <v>4.800000000000001</v>
+        <v>4.8</v>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>UConn -9.5</t>
+          <t>BYU -1.5</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>UConn -9.5</t>
+          <t>Iowa State -2.5</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>UConn -14.3</t>
+          <t>BYU -2.3</t>
         </is>
       </c>
       <c r="I8" t="n">
-        <v>-14.3</v>
+        <v>-2.3</v>
       </c>
       <c r="J8" t="n">
-        <v>-9.5</v>
+        <v>2.5</v>
       </c>
       <c r="K8" t="inlineStr"/>
       <c r="L8" t="inlineStr"/>
@@ -866,40 +866,40 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Texas Tech</t>
+          <t>Nebraska</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Oklahoma State</t>
+          <t>Northwestern</t>
         </is>
       </c>
       <c r="D9" t="n">
-        <v>3.1</v>
+        <v>8.199999999999999</v>
       </c>
       <c r="E9" t="n">
-        <v>4.299999999999997</v>
+        <v>4.6</v>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>Texas Tech -36.5</t>
+          <t>Nebraska -8.5</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>Texas Tech -36.5</t>
+          <t>Nebraska -7.5</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>Texas Tech -40.8</t>
+          <t>Nebraska -12.1</t>
         </is>
       </c>
       <c r="I9" t="n">
-        <v>40.8</v>
+        <v>12.1</v>
       </c>
       <c r="J9" t="n">
-        <v>36.5</v>
+        <v>7.5</v>
       </c>
       <c r="K9" t="inlineStr"/>
       <c r="L9" t="inlineStr"/>
@@ -916,40 +916,40 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Louisiana Tech</t>
+          <t>Rice</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Western Kentucky</t>
+          <t>UConn</t>
         </is>
       </c>
       <c r="D10" t="n">
-        <v>6.4</v>
+        <v>3.7</v>
       </c>
       <c r="E10" t="n">
-        <v>4.2</v>
+        <v>4.300000000000001</v>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>Louisiana Tech -3.0</t>
+          <t>UConn -9.5</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>Louisiana Tech -3</t>
+          <t>UConn -10</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>Louisiana Tech -7.2</t>
+          <t>UConn -14.3</t>
         </is>
       </c>
       <c r="I10" t="n">
-        <v>7.2</v>
+        <v>-14.3</v>
       </c>
       <c r="J10" t="n">
-        <v>3</v>
+        <v>-10</v>
       </c>
       <c r="K10" t="inlineStr"/>
       <c r="L10" t="inlineStr"/>
@@ -966,40 +966,40 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>North Carolina</t>
+          <t>Southern Miss</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Virginia</t>
+          <t>UL Monroe</t>
         </is>
       </c>
       <c r="D11" t="n">
-        <v>5.2</v>
+        <v>3.7</v>
       </c>
       <c r="E11" t="n">
-        <v>3.9</v>
+        <v>4.199999999999999</v>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>Virginia -10.0</t>
+          <t>Southern Miss -10.0</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>Virginia -10</t>
+          <t>Southern Miss -11.5</t>
         </is>
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>Virginia -13.9</t>
+          <t>Southern Miss -15.7</t>
         </is>
       </c>
       <c r="I11" t="n">
-        <v>-13.9</v>
+        <v>15.7</v>
       </c>
       <c r="J11" t="n">
-        <v>-10</v>
+        <v>11.5</v>
       </c>
       <c r="K11" t="inlineStr"/>
       <c r="L11" t="inlineStr"/>
@@ -1016,40 +1016,40 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Iowa State</t>
+          <t>North Carolina</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>BYU</t>
+          <t>Virginia</t>
         </is>
       </c>
       <c r="D12" t="n">
-        <v>9.199999999999999</v>
+        <v>5.2</v>
       </c>
       <c r="E12" t="n">
-        <v>3.8</v>
+        <v>3.9</v>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>BYU -1.5</t>
+          <t>Virginia -10.0</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>Iowa State -1.5</t>
+          <t>Virginia -10</t>
         </is>
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>BYU -2.3</t>
+          <t>Virginia -13.9</t>
         </is>
       </c>
       <c r="I12" t="n">
-        <v>-2.3</v>
+        <v>-13.9</v>
       </c>
       <c r="J12" t="n">
-        <v>1.5</v>
+        <v>-10</v>
       </c>
       <c r="K12" t="inlineStr"/>
       <c r="L12" t="inlineStr"/>
@@ -1066,40 +1066,40 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Nebraska</t>
+          <t>Central Michigan</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Northwestern</t>
+          <t>Massachusetts</t>
         </is>
       </c>
       <c r="D13" t="n">
-        <v>8.199999999999999</v>
+        <v>2.1</v>
       </c>
       <c r="E13" t="n">
-        <v>3.6</v>
+        <v>3.800000000000001</v>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>Nebraska -8.5</t>
+          <t>Central Michigan -16.5</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>Nebraska -8.5</t>
+          <t>Central Michigan -15.5</t>
         </is>
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>Nebraska -12.1</t>
+          <t>Central Michigan -19.3</t>
         </is>
       </c>
       <c r="I13" t="n">
-        <v>12.1</v>
+        <v>19.3</v>
       </c>
       <c r="J13" t="n">
-        <v>8.5</v>
+        <v>15.5</v>
       </c>
       <c r="K13" t="inlineStr"/>
       <c r="L13" t="inlineStr"/>
@@ -1116,40 +1116,40 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Washington State</t>
+          <t>Louisiana Tech</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>Toledo</t>
+          <t>Western Kentucky</t>
         </is>
       </c>
       <c r="D14" t="n">
-        <v>7</v>
+        <v>6.4</v>
       </c>
       <c r="E14" t="n">
-        <v>3.6</v>
+        <v>3.7</v>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>Toledo -1.5</t>
+          <t>Louisiana Tech -3.0</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>Toledo -1.5</t>
+          <t>Louisiana Tech -3.5</t>
         </is>
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>Toledo -5.1</t>
+          <t>Louisiana Tech -7.2</t>
         </is>
       </c>
       <c r="I14" t="n">
-        <v>-5.1</v>
+        <v>7.2</v>
       </c>
       <c r="J14" t="n">
-        <v>-1.5</v>
+        <v>3.5</v>
       </c>
       <c r="K14" t="inlineStr"/>
       <c r="L14" t="inlineStr"/>
@@ -1166,40 +1166,40 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Utah</t>
+          <t>New Mexico State</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Colorado</t>
+          <t>Missouri State</t>
         </is>
       </c>
       <c r="D15" t="n">
-        <v>7.8</v>
+        <v>5.2</v>
       </c>
       <c r="E15" t="n">
-        <v>3.5</v>
+        <v>3.3</v>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>Utah -14.5</t>
+          <t>Missouri State -1.5</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>Utah -14.5</t>
+          <t>Missouri State -1.5</t>
         </is>
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>Utah -18.0</t>
+          <t>New Mexico State -1.8</t>
         </is>
       </c>
       <c r="I15" t="n">
-        <v>18</v>
+        <v>1.8</v>
       </c>
       <c r="J15" t="n">
-        <v>14.5</v>
+        <v>-1.5</v>
       </c>
       <c r="K15" t="inlineStr"/>
       <c r="L15" t="inlineStr"/>
@@ -1216,40 +1216,40 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Michigan State</t>
+          <t>Oregon</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>Michigan</t>
+          <t>Wisconsin</t>
         </is>
       </c>
       <c r="D16" t="n">
-        <v>6.6</v>
+        <v>5.5</v>
       </c>
       <c r="E16" t="n">
-        <v>3.4</v>
+        <v>3.199999999999999</v>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>Michigan -8.5</t>
+          <t>Oregon -33.5</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>Michigan -12.5</t>
+          <t>Oregon -34.5</t>
         </is>
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>Michigan -15.9</t>
+          <t>Oregon -31.3</t>
         </is>
       </c>
       <c r="I16" t="n">
-        <v>-15.9</v>
+        <v>31.3</v>
       </c>
       <c r="J16" t="n">
-        <v>-12.5</v>
+        <v>34.5</v>
       </c>
       <c r="K16" t="inlineStr"/>
       <c r="L16" t="inlineStr"/>
@@ -1266,40 +1266,40 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>New Mexico State</t>
+          <t>Navy</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>Missouri State</t>
+          <t>Florida Atlantic</t>
         </is>
       </c>
       <c r="D17" t="n">
-        <v>5.2</v>
+        <v>4.5</v>
       </c>
       <c r="E17" t="n">
-        <v>3.3</v>
+        <v>3.199999999999999</v>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>Missouri State -1.5</t>
+          <t>Navy -14.5</t>
         </is>
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>Missouri State -1.5</t>
+          <t>Navy -14</t>
         </is>
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t>New Mexico State -1.8</t>
+          <t>Navy -17.2</t>
         </is>
       </c>
       <c r="I17" t="n">
-        <v>1.8</v>
+        <v>17.2</v>
       </c>
       <c r="J17" t="n">
-        <v>-1.5</v>
+        <v>14</v>
       </c>
       <c r="K17" t="inlineStr"/>
       <c r="L17" t="inlineStr"/>
@@ -1316,40 +1316,40 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Louisville</t>
+          <t>Mississippi State</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>Boston College</t>
+          <t>Texas</t>
         </is>
       </c>
       <c r="D18" t="n">
-        <v>4.6</v>
+        <v>8.699999999999999</v>
       </c>
       <c r="E18" t="n">
-        <v>3.100000000000001</v>
+        <v>3.1</v>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>Louisville -22.5</t>
+          <t>Texas -8.5</t>
         </is>
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>Louisville -22.5</t>
+          <t>Texas -6.5</t>
         </is>
       </c>
       <c r="H18" t="inlineStr">
         <is>
-          <t>Louisville -25.6</t>
+          <t>Texas -9.6</t>
         </is>
       </c>
       <c r="I18" t="n">
-        <v>25.6</v>
+        <v>-9.6</v>
       </c>
       <c r="J18" t="n">
-        <v>22.5</v>
+        <v>-6.5</v>
       </c>
       <c r="K18" t="inlineStr"/>
       <c r="L18" t="inlineStr"/>
@@ -1366,40 +1366,40 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Mississippi State</t>
+          <t>Tulsa</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>Texas</t>
+          <t>Temple</t>
         </is>
       </c>
       <c r="D19" t="n">
-        <v>8.699999999999999</v>
+        <v>4.3</v>
       </c>
       <c r="E19" t="n">
-        <v>3.1</v>
+        <v>2.699999999999999</v>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>Texas -8.5</t>
+          <t>Temple -6.0</t>
         </is>
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>Texas -6.5</t>
+          <t>Temple -6</t>
         </is>
       </c>
       <c r="H19" t="inlineStr">
         <is>
-          <t>Texas -9.6</t>
+          <t>Temple -8.7</t>
         </is>
       </c>
       <c r="I19" t="n">
-        <v>-9.6</v>
+        <v>-8.699999999999999</v>
       </c>
       <c r="J19" t="n">
-        <v>-6.5</v>
+        <v>-6</v>
       </c>
       <c r="K19" t="inlineStr"/>
       <c r="L19" t="inlineStr"/>
@@ -1416,40 +1416,40 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Central Michigan</t>
+          <t>Utah</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>Massachusetts</t>
+          <t>Colorado</t>
         </is>
       </c>
       <c r="D20" t="n">
-        <v>2.1</v>
+        <v>7.8</v>
       </c>
       <c r="E20" t="n">
-        <v>2.800000000000001</v>
+        <v>2.5</v>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>Central Michigan -16.5</t>
+          <t>Utah -14.5</t>
         </is>
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>Central Michigan -16.5</t>
+          <t>Utah -15.5</t>
         </is>
       </c>
       <c r="H20" t="inlineStr">
         <is>
-          <t>Central Michigan -19.3</t>
+          <t>Utah -18.0</t>
         </is>
       </c>
       <c r="I20" t="n">
-        <v>19.3</v>
+        <v>18</v>
       </c>
       <c r="J20" t="n">
-        <v>16.5</v>
+        <v>15.5</v>
       </c>
       <c r="K20" t="inlineStr"/>
       <c r="L20" t="inlineStr"/>
@@ -1466,40 +1466,40 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Navy</t>
+          <t>Kansas</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>Florida Atlantic</t>
+          <t>Kansas State</t>
         </is>
       </c>
       <c r="D21" t="n">
-        <v>4.5</v>
+        <v>9.1</v>
       </c>
       <c r="E21" t="n">
-        <v>2.699999999999999</v>
+        <v>2.5</v>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>Navy -14.5</t>
+          <t>Kansas State -4.0</t>
         </is>
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>Navy -14.5</t>
+          <t>Kansas -2.5</t>
         </is>
       </c>
       <c r="H21" t="inlineStr">
         <is>
-          <t>Navy -17.2</t>
+          <t>Kansas -5.0</t>
         </is>
       </c>
       <c r="I21" t="n">
-        <v>17.2</v>
+        <v>5</v>
       </c>
       <c r="J21" t="n">
-        <v>14.5</v>
+        <v>2.5</v>
       </c>
       <c r="K21" t="inlineStr"/>
       <c r="L21" t="inlineStr"/>
@@ -1516,40 +1516,40 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Tulsa</t>
+          <t>Wake Forest</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>Temple</t>
+          <t>SMU</t>
         </is>
       </c>
       <c r="D22" t="n">
-        <v>4.3</v>
+        <v>7.8</v>
       </c>
       <c r="E22" t="n">
-        <v>2.699999999999999</v>
+        <v>2.5</v>
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>Temple -6.0</t>
+          <t>SMU -4.5</t>
         </is>
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>Temple -6</t>
+          <t>SMU -4</t>
         </is>
       </c>
       <c r="H22" t="inlineStr">
         <is>
-          <t>Temple -8.7</t>
+          <t>SMU -6.5</t>
         </is>
       </c>
       <c r="I22" t="n">
-        <v>-8.699999999999999</v>
+        <v>-6.5</v>
       </c>
       <c r="J22" t="n">
-        <v>-6</v>
+        <v>-4</v>
       </c>
       <c r="K22" t="inlineStr"/>
       <c r="L22" t="inlineStr"/>
@@ -1566,40 +1566,40 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>Troy</t>
+          <t>Cincinnati</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>Louisiana</t>
+          <t>Baylor</t>
         </is>
       </c>
       <c r="D23" t="n">
-        <v>5.3</v>
+        <v>8.9</v>
       </c>
       <c r="E23" t="n">
-        <v>2.5</v>
+        <v>2.4</v>
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>Troy -8.5</t>
+          <t>Cincinnati -3.5</t>
         </is>
       </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t>Troy -8.5</t>
+          <t>Cincinnati -5.5</t>
         </is>
       </c>
       <c r="H23" t="inlineStr">
         <is>
-          <t>Troy -11.0</t>
+          <t>Cincinnati -7.9</t>
         </is>
       </c>
       <c r="I23" t="n">
-        <v>11</v>
+        <v>7.9</v>
       </c>
       <c r="J23" t="n">
-        <v>8.5</v>
+        <v>5.5</v>
       </c>
       <c r="K23" t="inlineStr"/>
       <c r="L23" t="inlineStr"/>
@@ -1616,40 +1616,40 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>Kansas</t>
+          <t>Michigan State</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>Kansas State</t>
+          <t>Michigan</t>
         </is>
       </c>
       <c r="D24" t="n">
-        <v>9.1</v>
+        <v>6.6</v>
       </c>
       <c r="E24" t="n">
-        <v>2.5</v>
+        <v>2.4</v>
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>Kansas State -4.0</t>
+          <t>Michigan -8.5</t>
         </is>
       </c>
       <c r="G24" t="inlineStr">
         <is>
-          <t>Kansas -2.5</t>
+          <t>Michigan -13.5</t>
         </is>
       </c>
       <c r="H24" t="inlineStr">
         <is>
-          <t>Kansas -5.0</t>
+          <t>Michigan -15.9</t>
         </is>
       </c>
       <c r="I24" t="n">
-        <v>5</v>
+        <v>-15.9</v>
       </c>
       <c r="J24" t="n">
-        <v>2.5</v>
+        <v>-13.5</v>
       </c>
       <c r="K24" t="inlineStr"/>
       <c r="L24" t="inlineStr"/>
@@ -1666,40 +1666,40 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>Pittsburgh</t>
+          <t>Texas Tech</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>NC State</t>
+          <t>Oklahoma State</t>
         </is>
       </c>
       <c r="D25" t="n">
-        <v>8.4</v>
+        <v>3.1</v>
       </c>
       <c r="E25" t="n">
-        <v>2.4</v>
+        <v>2.299999999999997</v>
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>Pittsburgh -7.5</t>
+          <t>Texas Tech -36.5</t>
         </is>
       </c>
       <c r="G25" t="inlineStr">
         <is>
-          <t>Pittsburgh -7.5</t>
+          <t>Texas Tech -38.5</t>
         </is>
       </c>
       <c r="H25" t="inlineStr">
         <is>
-          <t>Pittsburgh -9.9</t>
+          <t>Texas Tech -40.8</t>
         </is>
       </c>
       <c r="I25" t="n">
-        <v>9.9</v>
+        <v>40.8</v>
       </c>
       <c r="J25" t="n">
-        <v>7.5</v>
+        <v>38.5</v>
       </c>
       <c r="K25" t="inlineStr"/>
       <c r="L25" t="inlineStr"/>
@@ -1716,40 +1716,40 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>Cincinnati</t>
+          <t>Florida International</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>Baylor</t>
+          <t>Kennesaw State</t>
         </is>
       </c>
       <c r="D26" t="n">
-        <v>8.9</v>
+        <v>4.8</v>
       </c>
       <c r="E26" t="n">
-        <v>2.4</v>
+        <v>2.2</v>
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>Cincinnati -3.5</t>
+          <t>Kennesaw State -1.5</t>
         </is>
       </c>
       <c r="G26" t="inlineStr">
         <is>
-          <t>Cincinnati -5.5</t>
+          <t>Kennesaw State -1.5</t>
         </is>
       </c>
       <c r="H26" t="inlineStr">
         <is>
-          <t>Cincinnati -7.9</t>
+          <t>Kennesaw State -3.7</t>
         </is>
       </c>
       <c r="I26" t="n">
-        <v>7.9</v>
+        <v>-3.7</v>
       </c>
       <c r="J26" t="n">
-        <v>5.5</v>
+        <v>-1.5</v>
       </c>
       <c r="K26" t="inlineStr"/>
       <c r="L26" t="inlineStr"/>
@@ -1766,40 +1766,40 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>Northern Illinois</t>
+          <t>Louisville</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>Ball State</t>
+          <t>Boston College</t>
         </is>
       </c>
       <c r="D27" t="n">
-        <v>4.2</v>
+        <v>4.6</v>
       </c>
       <c r="E27" t="n">
-        <v>2.3</v>
+        <v>2.100000000000001</v>
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>Northern Illinois -6.0</t>
+          <t>Louisville -22.5</t>
         </is>
       </c>
       <c r="G27" t="inlineStr">
         <is>
-          <t>Northern Illinois -5</t>
+          <t>Louisville -23.5</t>
         </is>
       </c>
       <c r="H27" t="inlineStr">
         <is>
-          <t>Northern Illinois -7.3</t>
+          <t>Louisville -25.6</t>
         </is>
       </c>
       <c r="I27" t="n">
-        <v>7.3</v>
+        <v>25.6</v>
       </c>
       <c r="J27" t="n">
-        <v>5</v>
+        <v>23.5</v>
       </c>
       <c r="K27" t="inlineStr"/>
       <c r="L27" t="inlineStr"/>
@@ -1816,40 +1816,40 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>Florida International</t>
+          <t>LSU</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>Kennesaw State</t>
+          <t>Texas A&amp;M</t>
         </is>
       </c>
       <c r="D28" t="n">
-        <v>4.8</v>
+        <v>9.6</v>
       </c>
       <c r="E28" t="n">
-        <v>2.2</v>
+        <v>2.1</v>
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>Kennesaw State -1.5</t>
+          <t>LSU -5.5</t>
         </is>
       </c>
       <c r="G28" t="inlineStr">
         <is>
-          <t>Kennesaw State -1.5</t>
+          <t>Texas A&amp;M -2.5</t>
         </is>
       </c>
       <c r="H28" t="inlineStr">
         <is>
-          <t>Kennesaw State -3.7</t>
+          <t>Texas A&amp;M -0.4</t>
         </is>
       </c>
       <c r="I28" t="n">
-        <v>-3.7</v>
+        <v>-0.4</v>
       </c>
       <c r="J28" t="n">
-        <v>-1.5</v>
+        <v>-2.5</v>
       </c>
       <c r="K28" t="inlineStr"/>
       <c r="L28" t="inlineStr"/>
@@ -1866,40 +1866,40 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>Oregon</t>
+          <t>Arizona State</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>Wisconsin</t>
+          <t>Houston</t>
         </is>
       </c>
       <c r="D29" t="n">
-        <v>5.5</v>
+        <v>8.800000000000001</v>
       </c>
       <c r="E29" t="n">
-        <v>2.199999999999999</v>
+        <v>1.9</v>
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>Oregon -33.5</t>
+          <t>Arizona State -7.0</t>
         </is>
       </c>
       <c r="G29" t="inlineStr">
         <is>
-          <t>Oregon -33.5</t>
+          <t>Arizona State -8.5</t>
         </is>
       </c>
       <c r="H29" t="inlineStr">
         <is>
-          <t>Oregon -31.3</t>
+          <t>Arizona State -6.6</t>
         </is>
       </c>
       <c r="I29" t="n">
-        <v>31.3</v>
+        <v>6.6</v>
       </c>
       <c r="J29" t="n">
-        <v>33.5</v>
+        <v>8.5</v>
       </c>
       <c r="K29" t="inlineStr"/>
       <c r="L29" t="inlineStr"/>
@@ -1916,40 +1916,40 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>LSU</t>
+          <t>Arkansas</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>Texas A&amp;M</t>
+          <t>Auburn</t>
         </is>
       </c>
       <c r="D30" t="n">
-        <v>9.6</v>
+        <v>9.199999999999999</v>
       </c>
       <c r="E30" t="n">
-        <v>2.1</v>
+        <v>1.9</v>
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>LSU -5.5</t>
+          <t>Arkansas -1.5</t>
         </is>
       </c>
       <c r="G30" t="inlineStr">
         <is>
-          <t>Texas A&amp;M -2.5</t>
+          <t>Arkansas -1.5</t>
         </is>
       </c>
       <c r="H30" t="inlineStr">
         <is>
-          <t>Texas A&amp;M -0.4</t>
+          <t>Auburn -0.4</t>
         </is>
       </c>
       <c r="I30" t="n">
         <v>-0.4</v>
       </c>
       <c r="J30" t="n">
-        <v>-2.5</v>
+        <v>1.5</v>
       </c>
       <c r="K30" t="inlineStr"/>
       <c r="L30" t="inlineStr"/>
@@ -1966,40 +1966,40 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>Wake Forest</t>
+          <t>Arkansas State</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>SMU</t>
+          <t>Georgia Southern</t>
         </is>
       </c>
       <c r="D31" t="n">
-        <v>7.8</v>
+        <v>5.8</v>
       </c>
       <c r="E31" t="n">
-        <v>2</v>
+        <v>1.9</v>
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>SMU -4.5</t>
+          <t>Arkansas State -3.0</t>
         </is>
       </c>
       <c r="G31" t="inlineStr">
         <is>
-          <t>SMU -4.5</t>
+          <t>Arkansas State -3</t>
         </is>
       </c>
       <c r="H31" t="inlineStr">
         <is>
-          <t>SMU -6.5</t>
+          <t>Arkansas State -1.1</t>
         </is>
       </c>
       <c r="I31" t="n">
-        <v>-6.5</v>
+        <v>1.1</v>
       </c>
       <c r="J31" t="n">
-        <v>-4.5</v>
+        <v>3</v>
       </c>
       <c r="K31" t="inlineStr"/>
       <c r="L31" t="inlineStr"/>
@@ -2016,40 +2016,40 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>Arkansas</t>
+          <t>Northern Illinois</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>Auburn</t>
+          <t>Ball State</t>
         </is>
       </c>
       <c r="D32" t="n">
-        <v>9.199999999999999</v>
+        <v>4.2</v>
       </c>
       <c r="E32" t="n">
-        <v>1.9</v>
+        <v>1.8</v>
       </c>
       <c r="F32" t="inlineStr">
         <is>
-          <t>Arkansas -1.5</t>
+          <t>Northern Illinois -6.0</t>
         </is>
       </c>
       <c r="G32" t="inlineStr">
         <is>
-          <t>Arkansas -1.5</t>
+          <t>Northern Illinois -5.5</t>
         </is>
       </c>
       <c r="H32" t="inlineStr">
         <is>
-          <t>Auburn -0.4</t>
+          <t>Northern Illinois -7.3</t>
         </is>
       </c>
       <c r="I32" t="n">
-        <v>-0.4</v>
+        <v>7.3</v>
       </c>
       <c r="J32" t="n">
-        <v>1.5</v>
+        <v>5.5</v>
       </c>
       <c r="K32" t="inlineStr"/>
       <c r="L32" t="inlineStr"/>
@@ -2066,40 +2066,40 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>Georgia Tech</t>
+          <t>Wyoming</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>Syracuse</t>
+          <t>Colorado State</t>
         </is>
       </c>
       <c r="D33" t="n">
-        <v>6.9</v>
+        <v>6.7</v>
       </c>
       <c r="E33" t="n">
-        <v>1.5</v>
+        <v>1.7</v>
       </c>
       <c r="F33" t="inlineStr">
         <is>
-          <t>Georgia Tech -18.5</t>
+          <t>Wyoming -3.5</t>
         </is>
       </c>
       <c r="G33" t="inlineStr">
         <is>
-          <t>Georgia Tech -18.5</t>
+          <t>Wyoming -4.5</t>
         </is>
       </c>
       <c r="H33" t="inlineStr">
         <is>
-          <t>Georgia Tech -17.0</t>
+          <t>Wyoming -2.8</t>
         </is>
       </c>
       <c r="I33" t="n">
-        <v>17</v>
+        <v>2.8</v>
       </c>
       <c r="J33" t="n">
-        <v>18.5</v>
+        <v>4.5</v>
       </c>
       <c r="K33" t="inlineStr"/>
       <c r="L33" t="inlineStr"/>
@@ -2116,40 +2116,40 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>Old Dominion</t>
+          <t>Georgia Tech</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>App State</t>
+          <t>Syracuse</t>
         </is>
       </c>
       <c r="D34" t="n">
-        <v>5.1</v>
+        <v>6.9</v>
       </c>
       <c r="E34" t="n">
         <v>1.5</v>
       </c>
       <c r="F34" t="inlineStr">
         <is>
-          <t>Old Dominion -13.5</t>
+          <t>Georgia Tech -18.5</t>
         </is>
       </c>
       <c r="G34" t="inlineStr">
         <is>
-          <t>Old Dominion -13.5</t>
+          <t>Georgia Tech -18.5</t>
         </is>
       </c>
       <c r="H34" t="inlineStr">
         <is>
-          <t>Old Dominion -15.0</t>
+          <t>Georgia Tech -17.0</t>
         </is>
       </c>
       <c r="I34" t="n">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="J34" t="n">
-        <v>13.5</v>
+        <v>18.5</v>
       </c>
       <c r="K34" t="inlineStr"/>
       <c r="L34" t="inlineStr"/>
@@ -2166,40 +2166,40 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>Nevada</t>
+          <t>Troy</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>Boise State</t>
+          <t>Louisiana</t>
         </is>
       </c>
       <c r="D35" t="n">
-        <v>2.7</v>
+        <v>5.3</v>
       </c>
       <c r="E35" t="n">
         <v>1.5</v>
       </c>
       <c r="F35" t="inlineStr">
         <is>
-          <t>Boise State -21.5</t>
+          <t>Troy -8.5</t>
         </is>
       </c>
       <c r="G35" t="inlineStr">
         <is>
-          <t>Boise State -21.5</t>
+          <t>Troy -9.5</t>
         </is>
       </c>
       <c r="H35" t="inlineStr">
         <is>
-          <t>Boise State -23.0</t>
+          <t>Troy -11.0</t>
         </is>
       </c>
       <c r="I35" t="n">
-        <v>-23</v>
+        <v>11</v>
       </c>
       <c r="J35" t="n">
-        <v>-21.5</v>
+        <v>9.5</v>
       </c>
       <c r="K35" t="inlineStr"/>
       <c r="L35" t="inlineStr"/>
@@ -2216,40 +2216,40 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>New Mexico</t>
+          <t>Old Dominion</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>Utah State</t>
+          <t>App State</t>
         </is>
       </c>
       <c r="D36" t="n">
-        <v>7.5</v>
+        <v>5.1</v>
       </c>
       <c r="E36" t="n">
-        <v>1.4</v>
+        <v>1.5</v>
       </c>
       <c r="F36" t="inlineStr">
         <is>
-          <t>New Mexico -1.5</t>
+          <t>Old Dominion -13.5</t>
         </is>
       </c>
       <c r="G36" t="inlineStr">
         <is>
-          <t>New Mexico -1.5</t>
+          <t>Old Dominion -13.5</t>
         </is>
       </c>
       <c r="H36" t="inlineStr">
         <is>
-          <t>New Mexico -2.9</t>
+          <t>Old Dominion -15.0</t>
         </is>
       </c>
       <c r="I36" t="n">
-        <v>2.9</v>
+        <v>15</v>
       </c>
       <c r="J36" t="n">
-        <v>1.5</v>
+        <v>13.5</v>
       </c>
       <c r="K36" t="inlineStr"/>
       <c r="L36" t="inlineStr"/>
@@ -2266,40 +2266,40 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>Fresno State</t>
+          <t>Pittsburgh</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>San Diego State</t>
+          <t>NC State</t>
         </is>
       </c>
       <c r="D37" t="n">
-        <v>6.9</v>
+        <v>8.4</v>
       </c>
       <c r="E37" t="n">
-        <v>1.2</v>
+        <v>1.4</v>
       </c>
       <c r="F37" t="inlineStr">
         <is>
-          <t>San Diego State -2.5</t>
+          <t>Pittsburgh -7.5</t>
         </is>
       </c>
       <c r="G37" t="inlineStr">
         <is>
-          <t>San Diego State -2.5</t>
+          <t>Pittsburgh -8.5</t>
         </is>
       </c>
       <c r="H37" t="inlineStr">
         <is>
-          <t>San Diego State -3.7</t>
+          <t>Pittsburgh -9.9</t>
         </is>
       </c>
       <c r="I37" t="n">
-        <v>-3.7</v>
+        <v>9.9</v>
       </c>
       <c r="J37" t="n">
-        <v>-2.5</v>
+        <v>8.5</v>
       </c>
       <c r="K37" t="inlineStr"/>
       <c r="L37" t="inlineStr"/>
@@ -2316,40 +2316,40 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>Vanderbilt</t>
+          <t>Kent State</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>Missouri</t>
+          <t>Bowling Green</t>
         </is>
       </c>
       <c r="D38" t="n">
-        <v>9.699999999999999</v>
+        <v>2.8</v>
       </c>
       <c r="E38" t="n">
-        <v>1.2</v>
+        <v>1.300000000000001</v>
       </c>
       <c r="F38" t="inlineStr">
         <is>
-          <t>Vanderbilt -1.5</t>
+          <t>Bowling Green -10.0</t>
         </is>
       </c>
       <c r="G38" t="inlineStr">
         <is>
-          <t>Vanderbilt -3</t>
+          <t>Bowling Green -8.5</t>
         </is>
       </c>
       <c r="H38" t="inlineStr">
         <is>
-          <t>Vanderbilt -1.8</t>
+          <t>Bowling Green -9.8</t>
         </is>
       </c>
       <c r="I38" t="n">
-        <v>1.8</v>
+        <v>-9.800000000000001</v>
       </c>
       <c r="J38" t="n">
-        <v>3</v>
+        <v>-8.5</v>
       </c>
       <c r="K38" t="inlineStr"/>
       <c r="L38" t="inlineStr"/>
@@ -2366,40 +2366,40 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>Miami (OH)</t>
+          <t>Fresno State</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>Western Michigan</t>
+          <t>San Diego State</t>
         </is>
       </c>
       <c r="D39" t="n">
-        <v>7.1</v>
+        <v>6.9</v>
       </c>
       <c r="E39" t="n">
-        <v>1.1</v>
+        <v>1.2</v>
       </c>
       <c r="F39" t="inlineStr">
         <is>
-          <t>Miami (OH) -3.5</t>
+          <t>San Diego State -2.5</t>
         </is>
       </c>
       <c r="G39" t="inlineStr">
         <is>
-          <t>Miami (OH) -3.5</t>
+          <t>San Diego State -2.5</t>
         </is>
       </c>
       <c r="H39" t="inlineStr">
         <is>
-          <t>Miami (OH) -2.4</t>
+          <t>San Diego State -3.7</t>
         </is>
       </c>
       <c r="I39" t="n">
-        <v>2.4</v>
+        <v>-3.7</v>
       </c>
       <c r="J39" t="n">
-        <v>3.5</v>
+        <v>-2.5</v>
       </c>
       <c r="K39" t="inlineStr"/>
       <c r="L39" t="inlineStr"/>
@@ -2516,40 +2516,40 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>Oklahoma</t>
+          <t>Georgia State</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>Ole Miss</t>
+          <t>South Alabama</t>
         </is>
       </c>
       <c r="D42" t="n">
-        <v>9.699999999999999</v>
+        <v>3.5</v>
       </c>
       <c r="E42" t="n">
-        <v>0.7999999999999998</v>
+        <v>0.7000000000000002</v>
       </c>
       <c r="F42" t="inlineStr">
         <is>
-          <t>Oklahoma -2.5</t>
+          <t>South Alabama -6.5</t>
         </is>
       </c>
       <c r="G42" t="inlineStr">
         <is>
-          <t>Oklahoma -3.5</t>
+          <t>South Alabama -6.5</t>
         </is>
       </c>
       <c r="H42" t="inlineStr">
         <is>
-          <t>Oklahoma -4.3</t>
+          <t>South Alabama -7.2</t>
         </is>
       </c>
       <c r="I42" t="n">
-        <v>4.3</v>
+        <v>-7.2</v>
       </c>
       <c r="J42" t="n">
-        <v>3.5</v>
+        <v>-6.5</v>
       </c>
       <c r="K42" t="inlineStr"/>
       <c r="L42" t="inlineStr"/>
@@ -2566,40 +2566,40 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>Georgia State</t>
+          <t>Vanderbilt</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>South Alabama</t>
+          <t>Missouri</t>
         </is>
       </c>
       <c r="D43" t="n">
-        <v>3.5</v>
+        <v>9.699999999999999</v>
       </c>
       <c r="E43" t="n">
-        <v>0.7000000000000002</v>
+        <v>0.7</v>
       </c>
       <c r="F43" t="inlineStr">
         <is>
-          <t>South Alabama -6.5</t>
+          <t>Vanderbilt -1.5</t>
         </is>
       </c>
       <c r="G43" t="inlineStr">
         <is>
-          <t>South Alabama -6.5</t>
+          <t>Vanderbilt -2.5</t>
         </is>
       </c>
       <c r="H43" t="inlineStr">
         <is>
-          <t>South Alabama -7.2</t>
+          <t>Vanderbilt -1.8</t>
         </is>
       </c>
       <c r="I43" t="n">
-        <v>-7.2</v>
+        <v>1.8</v>
       </c>
       <c r="J43" t="n">
-        <v>-6.5</v>
+        <v>2.5</v>
       </c>
       <c r="K43" t="inlineStr"/>
       <c r="L43" t="inlineStr"/>
@@ -2666,40 +2666,40 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>Arizona State</t>
+          <t>Charlotte</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>Houston</t>
+          <t>North Texas</t>
         </is>
       </c>
       <c r="D45" t="n">
-        <v>8.800000000000001</v>
+        <v>1.9</v>
       </c>
       <c r="E45" t="n">
-        <v>0.4000000000000004</v>
+        <v>0.6000000000000014</v>
       </c>
       <c r="F45" t="inlineStr">
         <is>
-          <t>Arizona State -7.0</t>
+          <t>North Texas -27.5</t>
         </is>
       </c>
       <c r="G45" t="inlineStr">
         <is>
-          <t>Arizona State -7</t>
+          <t>North Texas -27.5</t>
         </is>
       </c>
       <c r="H45" t="inlineStr">
         <is>
-          <t>Arizona State -6.6</t>
+          <t>North Texas -28.1</t>
         </is>
       </c>
       <c r="I45" t="n">
-        <v>6.6</v>
+        <v>-28.1</v>
       </c>
       <c r="J45" t="n">
-        <v>7</v>
+        <v>-27.5</v>
       </c>
       <c r="K45" t="inlineStr"/>
       <c r="L45" t="inlineStr"/>
@@ -2716,40 +2716,40 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>Kentucky</t>
+          <t>Virginia Tech</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>Tennessee</t>
+          <t>California</t>
         </is>
       </c>
       <c r="D46" t="n">
-        <v>8.199999999999999</v>
+        <v>7.8</v>
       </c>
       <c r="E46" t="n">
-        <v>0.4000000000000004</v>
+        <v>0.5</v>
       </c>
       <c r="F46" t="inlineStr">
         <is>
-          <t>Tennessee -9.5</t>
+          <t>Virginia Tech -2.5</t>
         </is>
       </c>
       <c r="G46" t="inlineStr">
         <is>
-          <t>Tennessee -9.5</t>
+          <t>Virginia Tech -4</t>
         </is>
       </c>
       <c r="H46" t="inlineStr">
         <is>
-          <t>Tennessee -9.1</t>
+          <t>Virginia Tech -3.5</t>
         </is>
       </c>
       <c r="I46" t="n">
-        <v>-9.1</v>
+        <v>3.5</v>
       </c>
       <c r="J46" t="n">
-        <v>-9.5</v>
+        <v>4</v>
       </c>
       <c r="K46" t="inlineStr"/>
       <c r="L46" t="inlineStr"/>
@@ -2766,40 +2766,40 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>West Virginia</t>
+          <t>Nevada</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>TCU</t>
+          <t>Boise State</t>
         </is>
       </c>
       <c r="D47" t="n">
-        <v>5.8</v>
+        <v>2.7</v>
       </c>
       <c r="E47" t="n">
-        <v>0.4000000000000004</v>
+        <v>0.5</v>
       </c>
       <c r="F47" t="inlineStr">
         <is>
-          <t>TCU -14.5</t>
+          <t>Boise State -21.5</t>
         </is>
       </c>
       <c r="G47" t="inlineStr">
         <is>
-          <t>TCU -14.5</t>
+          <t>Boise State -22.5</t>
         </is>
       </c>
       <c r="H47" t="inlineStr">
         <is>
-          <t>TCU -14.1</t>
+          <t>Boise State -23.0</t>
         </is>
       </c>
       <c r="I47" t="n">
-        <v>-14.1</v>
+        <v>-23</v>
       </c>
       <c r="J47" t="n">
-        <v>-14.5</v>
+        <v>-22.5</v>
       </c>
       <c r="K47" t="inlineStr"/>
       <c r="L47" t="inlineStr"/>
@@ -2816,40 +2816,40 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>Kent State</t>
+          <t>Kentucky</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>Bowling Green</t>
+          <t>Tennessee</t>
         </is>
       </c>
       <c r="D48" t="n">
-        <v>2.8</v>
+        <v>8.199999999999999</v>
       </c>
       <c r="E48" t="n">
-        <v>0.1999999999999993</v>
+        <v>0.4000000000000004</v>
       </c>
       <c r="F48" t="inlineStr">
         <is>
-          <t>Bowling Green -10.0</t>
+          <t>Tennessee -9.5</t>
         </is>
       </c>
       <c r="G48" t="inlineStr">
         <is>
-          <t>Bowling Green -10</t>
+          <t>Tennessee -9.5</t>
         </is>
       </c>
       <c r="H48" t="inlineStr">
         <is>
-          <t>Bowling Green -9.8</t>
+          <t>Tennessee -9.1</t>
         </is>
       </c>
       <c r="I48" t="n">
-        <v>-9.800000000000001</v>
+        <v>-9.1</v>
       </c>
       <c r="J48" t="n">
-        <v>-10</v>
+        <v>-9.5</v>
       </c>
       <c r="K48" t="inlineStr"/>
       <c r="L48" t="inlineStr"/>
@@ -2866,40 +2866,40 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>Charlotte</t>
+          <t>West Virginia</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>North Texas</t>
+          <t>TCU</t>
         </is>
       </c>
       <c r="D49" t="n">
-        <v>1.9</v>
+        <v>5.8</v>
       </c>
       <c r="E49" t="n">
-        <v>0.1000000000000014</v>
+        <v>0.4000000000000004</v>
       </c>
       <c r="F49" t="inlineStr">
         <is>
-          <t>North Texas -27.5</t>
+          <t>TCU -14.5</t>
         </is>
       </c>
       <c r="G49" t="inlineStr">
         <is>
-          <t>North Texas -28</t>
+          <t>TCU -14.5</t>
         </is>
       </c>
       <c r="H49" t="inlineStr">
         <is>
-          <t>North Texas -28.1</t>
+          <t>TCU -14.1</t>
         </is>
       </c>
       <c r="I49" t="n">
-        <v>-28.1</v>
+        <v>-14.1</v>
       </c>
       <c r="J49" t="n">
-        <v>-28</v>
+        <v>-14.5</v>
       </c>
       <c r="K49" t="inlineStr"/>
       <c r="L49" t="inlineStr"/>
@@ -2928,7 +2928,7 @@
         <v>9.5</v>
       </c>
       <c r="E50" t="n">
-        <v>0.1000000000000001</v>
+        <v>0.3999999999999999</v>
       </c>
       <c r="F50" t="inlineStr">
         <is>
@@ -2937,7 +2937,7 @@
       </c>
       <c r="G50" t="inlineStr">
         <is>
-          <t>Washington -3.5</t>
+          <t>Washington -4</t>
         </is>
       </c>
       <c r="H50" t="inlineStr">
@@ -2949,7 +2949,7 @@
         <v>3.6</v>
       </c>
       <c r="J50" t="n">
-        <v>3.5</v>
+        <v>4</v>
       </c>
       <c r="K50" t="inlineStr"/>
       <c r="L50" t="inlineStr"/>
@@ -2966,40 +2966,40 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>Miami</t>
+          <t>New Mexico</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>Stanford</t>
+          <t>Utah State</t>
         </is>
       </c>
       <c r="D51" t="n">
-        <v>4.5</v>
+        <v>7.5</v>
       </c>
       <c r="E51" t="n">
-        <v>0</v>
+        <v>0.3999999999999999</v>
       </c>
       <c r="F51" t="inlineStr">
         <is>
-          <t>Miami -30.5</t>
+          <t>New Mexico -1.5</t>
         </is>
       </c>
       <c r="G51" t="inlineStr">
         <is>
-          <t>Miami -30.5</t>
+          <t>New Mexico -2.5</t>
         </is>
       </c>
       <c r="H51" t="inlineStr">
         <is>
-          <t>Miami -30.5</t>
+          <t>New Mexico -2.9</t>
         </is>
       </c>
       <c r="I51" t="n">
-        <v>30.5</v>
+        <v>2.9</v>
       </c>
       <c r="J51" t="n">
-        <v>30.5</v>
+        <v>2.5</v>
       </c>
       <c r="K51" t="inlineStr"/>
       <c r="L51" t="inlineStr"/>
@@ -3016,40 +3016,40 @@
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>Virginia Tech</t>
+          <t>Oklahoma</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>California</t>
+          <t>Ole Miss</t>
         </is>
       </c>
       <c r="D52" t="n">
-        <v>7.8</v>
+        <v>9.699999999999999</v>
       </c>
       <c r="E52" t="n">
-        <v>0</v>
+        <v>0.2999999999999998</v>
       </c>
       <c r="F52" t="inlineStr">
         <is>
-          <t>Virginia Tech -2.5</t>
+          <t>Oklahoma -2.5</t>
         </is>
       </c>
       <c r="G52" t="inlineStr">
         <is>
-          <t>Virginia Tech -3.5</t>
+          <t>Oklahoma -4</t>
         </is>
       </c>
       <c r="H52" t="inlineStr">
         <is>
-          <t>Virginia Tech -3.5</t>
+          <t>Oklahoma -4.3</t>
         </is>
       </c>
       <c r="I52" t="n">
-        <v>3.5</v>
+        <v>4.3</v>
       </c>
       <c r="J52" t="n">
-        <v>3.5</v>
+        <v>4</v>
       </c>
       <c r="K52" t="inlineStr"/>
       <c r="L52" t="inlineStr"/>
@@ -3060,6 +3060,106 @@
         <v>0</v>
       </c>
     </row>
+    <row r="53">
+      <c r="A53" s="1" t="n">
+        <v>51</v>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>Miami (OH)</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>Western Michigan</t>
+        </is>
+      </c>
+      <c r="D53" t="n">
+        <v>7.1</v>
+      </c>
+      <c r="E53" t="n">
+        <v>0.1000000000000001</v>
+      </c>
+      <c r="F53" t="inlineStr">
+        <is>
+          <t>Miami (OH) -3.5</t>
+        </is>
+      </c>
+      <c r="G53" t="inlineStr">
+        <is>
+          <t>Miami (OH) -2.5</t>
+        </is>
+      </c>
+      <c r="H53" t="inlineStr">
+        <is>
+          <t>Miami (OH) -2.4</t>
+        </is>
+      </c>
+      <c r="I53" t="n">
+        <v>2.4</v>
+      </c>
+      <c r="J53" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="K53" t="inlineStr"/>
+      <c r="L53" t="inlineStr"/>
+      <c r="M53" t="inlineStr"/>
+      <c r="N53" t="inlineStr"/>
+      <c r="O53" t="inlineStr"/>
+      <c r="P53" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" s="1" t="n">
+        <v>52</v>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>Miami</t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>Stanford</t>
+        </is>
+      </c>
+      <c r="D54" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="E54" t="n">
+        <v>0</v>
+      </c>
+      <c r="F54" t="inlineStr">
+        <is>
+          <t>Miami -30.5</t>
+        </is>
+      </c>
+      <c r="G54" t="inlineStr">
+        <is>
+          <t>Miami -30.5</t>
+        </is>
+      </c>
+      <c r="H54" t="inlineStr">
+        <is>
+          <t>Miami -30.5</t>
+        </is>
+      </c>
+      <c r="I54" t="n">
+        <v>30.5</v>
+      </c>
+      <c r="J54" t="n">
+        <v>30.5</v>
+      </c>
+      <c r="K54" t="inlineStr"/>
+      <c r="L54" t="inlineStr"/>
+      <c r="M54" t="inlineStr"/>
+      <c r="N54" t="inlineStr"/>
+      <c r="O54" t="inlineStr"/>
+      <c r="P54" t="n">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
updating the necessary graphics
</commit_message>
<xml_diff>
--- a/PEAR/PEAR Football/y2025/Spreads/spreads_tracker_week9.xlsx
+++ b/PEAR/PEAR Football/y2025/Spreads/spreads_tracker_week9.xlsx
@@ -516,40 +516,40 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Washington State</t>
+          <t>Delaware</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Toledo</t>
+          <t>Middle Tennessee</t>
         </is>
       </c>
       <c r="D2" t="n">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="E2" t="n">
-        <v>6.6</v>
+        <v>6.9</v>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>Toledo -1.5</t>
+          <t>Delaware -10.0</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>Washington State -1.5</t>
+          <t>Delaware -8.5</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>Toledo -5.1</t>
+          <t>Delaware -15.4</t>
         </is>
       </c>
       <c r="I2" t="n">
-        <v>-5.1</v>
+        <v>15.4</v>
       </c>
       <c r="J2" t="n">
-        <v>1.5</v>
+        <v>8.5</v>
       </c>
       <c r="K2" t="inlineStr"/>
       <c r="L2" t="inlineStr"/>
@@ -578,16 +578,16 @@
         <v>9.300000000000001</v>
       </c>
       <c r="E3" t="n">
-        <v>6.4</v>
+        <v>6.9</v>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>Memphis -3.0</t>
+          <t>South Florida -3.5</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>South Florida -3.5</t>
+          <t>South Florida -4.0</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
@@ -599,7 +599,7 @@
         <v>2.9</v>
       </c>
       <c r="J3" t="n">
-        <v>-3.5</v>
+        <v>-4</v>
       </c>
       <c r="K3" t="inlineStr"/>
       <c r="L3" t="inlineStr"/>
@@ -616,40 +616,40 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Delaware</t>
+          <t>Washington State</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Middle Tennessee</t>
+          <t>Toledo</t>
         </is>
       </c>
       <c r="D4" t="n">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="E4" t="n">
-        <v>5.4</v>
+        <v>6.6</v>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>Delaware -10.5</t>
+          <t>Washington State -1.5</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>Delaware -10</t>
+          <t>Washington State -1.5</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>Delaware -15.4</t>
+          <t>Toledo -5.1</t>
         </is>
       </c>
       <c r="I4" t="n">
-        <v>15.4</v>
+        <v>-5.1</v>
       </c>
       <c r="J4" t="n">
-        <v>10</v>
+        <v>1.5</v>
       </c>
       <c r="K4" t="inlineStr"/>
       <c r="L4" t="inlineStr"/>
@@ -678,16 +678,16 @@
         <v>3.1</v>
       </c>
       <c r="E5" t="n">
-        <v>5</v>
+        <v>6.5</v>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>Buffalo -10.0</t>
+          <t>Buffalo -11.0</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>Buffalo -10.5</t>
+          <t>Buffalo -9.0</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
@@ -699,7 +699,7 @@
         <v>15.5</v>
       </c>
       <c r="J5" t="n">
-        <v>10.5</v>
+        <v>9</v>
       </c>
       <c r="K5" t="inlineStr"/>
       <c r="L5" t="inlineStr"/>
@@ -716,40 +716,40 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Iowa</t>
+          <t>Nebraska</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Minnesota</t>
+          <t>Northwestern</t>
         </is>
       </c>
       <c r="D6" t="n">
-        <v>8.5</v>
+        <v>8.199999999999999</v>
       </c>
       <c r="E6" t="n">
-        <v>4.9</v>
+        <v>5.6</v>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>Iowa -7.0</t>
+          <t>Nebraska -7.5</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>Iowa -7.5</t>
+          <t>Nebraska -6.5</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>Iowa -12.4</t>
+          <t>Nebraska -12.1</t>
         </is>
       </c>
       <c r="I6" t="n">
-        <v>12.4</v>
+        <v>12.1</v>
       </c>
       <c r="J6" t="n">
-        <v>7.5</v>
+        <v>6.5</v>
       </c>
       <c r="K6" t="inlineStr"/>
       <c r="L6" t="inlineStr"/>
@@ -778,16 +778,16 @@
         <v>6.1</v>
       </c>
       <c r="E7" t="n">
-        <v>4.800000000000001</v>
+        <v>5.300000000000001</v>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>Indiana -23.5</t>
+          <t>Indiana -24.5</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>Indiana -24.5</t>
+          <t>Indiana -24.0</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
@@ -799,7 +799,7 @@
         <v>29.3</v>
       </c>
       <c r="J7" t="n">
-        <v>24.5</v>
+        <v>24</v>
       </c>
       <c r="K7" t="inlineStr"/>
       <c r="L7" t="inlineStr"/>
@@ -832,7 +832,7 @@
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>BYU -1.5</t>
+          <t>Iowa State -2.0</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
@@ -866,40 +866,40 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Nebraska</t>
+          <t>Central Michigan</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Northwestern</t>
+          <t>Massachusetts</t>
         </is>
       </c>
       <c r="D9" t="n">
-        <v>8.199999999999999</v>
+        <v>2.1</v>
       </c>
       <c r="E9" t="n">
-        <v>4.6</v>
+        <v>4.300000000000001</v>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>Nebraska -8.5</t>
+          <t>Central Michigan -16.0</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>Nebraska -7.5</t>
+          <t>Central Michigan -15.0</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>Nebraska -12.1</t>
+          <t>Central Michigan -19.3</t>
         </is>
       </c>
       <c r="I9" t="n">
-        <v>12.1</v>
+        <v>19.3</v>
       </c>
       <c r="J9" t="n">
-        <v>7.5</v>
+        <v>15</v>
       </c>
       <c r="K9" t="inlineStr"/>
       <c r="L9" t="inlineStr"/>
@@ -916,40 +916,40 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Rice</t>
+          <t>Iowa</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>UConn</t>
+          <t>Minnesota</t>
         </is>
       </c>
       <c r="D10" t="n">
-        <v>3.7</v>
+        <v>8.5</v>
       </c>
       <c r="E10" t="n">
-        <v>4.300000000000001</v>
+        <v>3.9</v>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>UConn -9.5</t>
+          <t>Iowa -7.5</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>UConn -10</t>
+          <t>Iowa -8.5</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>UConn -14.3</t>
+          <t>Iowa -12.4</t>
         </is>
       </c>
       <c r="I10" t="n">
-        <v>-14.3</v>
+        <v>12.4</v>
       </c>
       <c r="J10" t="n">
-        <v>-10</v>
+        <v>8.5</v>
       </c>
       <c r="K10" t="inlineStr"/>
       <c r="L10" t="inlineStr"/>
@@ -966,40 +966,40 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Southern Miss</t>
+          <t>North Carolina</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>UL Monroe</t>
+          <t>Virginia</t>
         </is>
       </c>
       <c r="D11" t="n">
-        <v>3.7</v>
+        <v>5.2</v>
       </c>
       <c r="E11" t="n">
-        <v>4.199999999999999</v>
+        <v>3.9</v>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>Southern Miss -10.0</t>
+          <t>Virginia -9.0</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>Southern Miss -11.5</t>
+          <t>Virginia -10.0</t>
         </is>
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>Southern Miss -15.7</t>
+          <t>Virginia -13.9</t>
         </is>
       </c>
       <c r="I11" t="n">
-        <v>15.7</v>
+        <v>-13.9</v>
       </c>
       <c r="J11" t="n">
-        <v>11.5</v>
+        <v>-10</v>
       </c>
       <c r="K11" t="inlineStr"/>
       <c r="L11" t="inlineStr"/>
@@ -1016,40 +1016,40 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>North Carolina</t>
+          <t>Rice</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Virginia</t>
+          <t>UConn</t>
         </is>
       </c>
       <c r="D12" t="n">
-        <v>5.2</v>
+        <v>3.7</v>
       </c>
       <c r="E12" t="n">
-        <v>3.9</v>
+        <v>3.800000000000001</v>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>Virginia -10.0</t>
+          <t>UConn -10.0</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>Virginia -10</t>
+          <t>UConn -10.5</t>
         </is>
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>Virginia -13.9</t>
+          <t>UConn -14.3</t>
         </is>
       </c>
       <c r="I12" t="n">
-        <v>-13.9</v>
+        <v>-14.3</v>
       </c>
       <c r="J12" t="n">
-        <v>-10</v>
+        <v>-10.5</v>
       </c>
       <c r="K12" t="inlineStr"/>
       <c r="L12" t="inlineStr"/>
@@ -1066,40 +1066,40 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Central Michigan</t>
+          <t>New Mexico State</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Massachusetts</t>
+          <t>Missouri State</t>
         </is>
       </c>
       <c r="D13" t="n">
-        <v>2.1</v>
+        <v>5.2</v>
       </c>
       <c r="E13" t="n">
-        <v>3.800000000000001</v>
+        <v>3.8</v>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>Central Michigan -16.5</t>
+          <t>Missouri State -2.0</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>Central Michigan -15.5</t>
+          <t>Missouri State -2.0</t>
         </is>
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>Central Michigan -19.3</t>
+          <t>New Mexico State -1.8</t>
         </is>
       </c>
       <c r="I13" t="n">
-        <v>19.3</v>
+        <v>1.8</v>
       </c>
       <c r="J13" t="n">
-        <v>15.5</v>
+        <v>-2</v>
       </c>
       <c r="K13" t="inlineStr"/>
       <c r="L13" t="inlineStr"/>
@@ -1166,40 +1166,40 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>New Mexico State</t>
+          <t>Southern Miss</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Missouri State</t>
+          <t>UL Monroe</t>
         </is>
       </c>
       <c r="D15" t="n">
-        <v>5.2</v>
+        <v>3.7</v>
       </c>
       <c r="E15" t="n">
-        <v>3.3</v>
+        <v>3.699999999999999</v>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>Missouri State -1.5</t>
+          <t>Southern Miss -11.5</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>Missouri State -1.5</t>
+          <t>Southern Miss -12.0</t>
         </is>
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>New Mexico State -1.8</t>
+          <t>Southern Miss -15.7</t>
         </is>
       </c>
       <c r="I15" t="n">
-        <v>1.8</v>
+        <v>15.7</v>
       </c>
       <c r="J15" t="n">
-        <v>-1.5</v>
+        <v>12</v>
       </c>
       <c r="K15" t="inlineStr"/>
       <c r="L15" t="inlineStr"/>
@@ -1216,40 +1216,40 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Oregon</t>
+          <t>Wyoming</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>Wisconsin</t>
+          <t>Colorado State</t>
         </is>
       </c>
       <c r="D16" t="n">
-        <v>5.5</v>
+        <v>6.7</v>
       </c>
       <c r="E16" t="n">
-        <v>3.199999999999999</v>
+        <v>3.2</v>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>Oregon -33.5</t>
+          <t>Wyoming -5.0</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>Oregon -34.5</t>
+          <t>Wyoming -6.0</t>
         </is>
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>Oregon -31.3</t>
+          <t>Wyoming -2.8</t>
         </is>
       </c>
       <c r="I16" t="n">
-        <v>31.3</v>
+        <v>2.8</v>
       </c>
       <c r="J16" t="n">
-        <v>34.5</v>
+        <v>6</v>
       </c>
       <c r="K16" t="inlineStr"/>
       <c r="L16" t="inlineStr"/>
@@ -1266,40 +1266,40 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Navy</t>
+          <t>Oregon</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>Florida Atlantic</t>
+          <t>Wisconsin</t>
         </is>
       </c>
       <c r="D17" t="n">
-        <v>4.5</v>
+        <v>5.5</v>
       </c>
       <c r="E17" t="n">
         <v>3.199999999999999</v>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>Navy -14.5</t>
+          <t>Oregon -34.0</t>
         </is>
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>Navy -14</t>
+          <t>Oregon -34.5</t>
         </is>
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t>Navy -17.2</t>
+          <t>Oregon -31.3</t>
         </is>
       </c>
       <c r="I17" t="n">
-        <v>17.2</v>
+        <v>31.3</v>
       </c>
       <c r="J17" t="n">
-        <v>14</v>
+        <v>34.5</v>
       </c>
       <c r="K17" t="inlineStr"/>
       <c r="L17" t="inlineStr"/>
@@ -1332,7 +1332,7 @@
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>Texas -8.5</t>
+          <t>Texas -6.5</t>
         </is>
       </c>
       <c r="G18" t="inlineStr">
@@ -1366,40 +1366,40 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Tulsa</t>
+          <t>Utah</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>Temple</t>
+          <t>Colorado</t>
         </is>
       </c>
       <c r="D19" t="n">
-        <v>4.3</v>
+        <v>7.8</v>
       </c>
       <c r="E19" t="n">
-        <v>2.699999999999999</v>
+        <v>3</v>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>Temple -6.0</t>
+          <t>Utah -15.5</t>
         </is>
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>Temple -6</t>
+          <t>Utah -15.0</t>
         </is>
       </c>
       <c r="H19" t="inlineStr">
         <is>
-          <t>Temple -8.7</t>
+          <t>Utah -18.0</t>
         </is>
       </c>
       <c r="I19" t="n">
-        <v>-8.699999999999999</v>
+        <v>18</v>
       </c>
       <c r="J19" t="n">
-        <v>-6</v>
+        <v>15</v>
       </c>
       <c r="K19" t="inlineStr"/>
       <c r="L19" t="inlineStr"/>
@@ -1416,40 +1416,40 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Utah</t>
+          <t>Wake Forest</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>Colorado</t>
+          <t>SMU</t>
         </is>
       </c>
       <c r="D20" t="n">
         <v>7.8</v>
       </c>
       <c r="E20" t="n">
-        <v>2.5</v>
+        <v>3</v>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>Utah -14.5</t>
+          <t>SMU -3.5</t>
         </is>
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>Utah -15.5</t>
+          <t>SMU -3.5</t>
         </is>
       </c>
       <c r="H20" t="inlineStr">
         <is>
-          <t>Utah -18.0</t>
+          <t>SMU -6.5</t>
         </is>
       </c>
       <c r="I20" t="n">
-        <v>18</v>
+        <v>-6.5</v>
       </c>
       <c r="J20" t="n">
-        <v>15.5</v>
+        <v>-3.5</v>
       </c>
       <c r="K20" t="inlineStr"/>
       <c r="L20" t="inlineStr"/>
@@ -1466,40 +1466,40 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Kansas</t>
+          <t>Pittsburgh</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>Kansas State</t>
+          <t>NC State</t>
         </is>
       </c>
       <c r="D21" t="n">
-        <v>9.1</v>
+        <v>8.4</v>
       </c>
       <c r="E21" t="n">
-        <v>2.5</v>
+        <v>2.9</v>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>Kansas State -4.0</t>
+          <t>Pittsburgh -8.5</t>
         </is>
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>Kansas -2.5</t>
+          <t>Pittsburgh -7.0</t>
         </is>
       </c>
       <c r="H21" t="inlineStr">
         <is>
-          <t>Kansas -5.0</t>
+          <t>Pittsburgh -9.9</t>
         </is>
       </c>
       <c r="I21" t="n">
-        <v>5</v>
+        <v>9.9</v>
       </c>
       <c r="J21" t="n">
-        <v>2.5</v>
+        <v>7</v>
       </c>
       <c r="K21" t="inlineStr"/>
       <c r="L21" t="inlineStr"/>
@@ -1516,40 +1516,40 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Wake Forest</t>
+          <t>Tulsa</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>SMU</t>
+          <t>Temple</t>
         </is>
       </c>
       <c r="D22" t="n">
-        <v>7.8</v>
+        <v>4.3</v>
       </c>
       <c r="E22" t="n">
-        <v>2.5</v>
+        <v>2.699999999999999</v>
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>SMU -4.5</t>
+          <t>Temple -6.0</t>
         </is>
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>SMU -4</t>
+          <t>Temple -6.0</t>
         </is>
       </c>
       <c r="H22" t="inlineStr">
         <is>
-          <t>SMU -6.5</t>
+          <t>Temple -8.7</t>
         </is>
       </c>
       <c r="I22" t="n">
-        <v>-6.5</v>
+        <v>-8.699999999999999</v>
       </c>
       <c r="J22" t="n">
-        <v>-4</v>
+        <v>-6</v>
       </c>
       <c r="K22" t="inlineStr"/>
       <c r="L22" t="inlineStr"/>
@@ -1566,40 +1566,40 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>Cincinnati</t>
+          <t>Troy</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>Baylor</t>
+          <t>Louisiana</t>
         </is>
       </c>
       <c r="D23" t="n">
-        <v>8.9</v>
+        <v>5.3</v>
       </c>
       <c r="E23" t="n">
-        <v>2.4</v>
+        <v>2.5</v>
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>Cincinnati -3.5</t>
+          <t>Troy -9.5</t>
         </is>
       </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t>Cincinnati -5.5</t>
+          <t>Troy -8.5</t>
         </is>
       </c>
       <c r="H23" t="inlineStr">
         <is>
-          <t>Cincinnati -7.9</t>
+          <t>Troy -11.0</t>
         </is>
       </c>
       <c r="I23" t="n">
-        <v>7.9</v>
+        <v>11</v>
       </c>
       <c r="J23" t="n">
-        <v>5.5</v>
+        <v>8.5</v>
       </c>
       <c r="K23" t="inlineStr"/>
       <c r="L23" t="inlineStr"/>
@@ -1616,40 +1616,40 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>Michigan State</t>
+          <t>Cincinnati</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>Michigan</t>
+          <t>Baylor</t>
         </is>
       </c>
       <c r="D24" t="n">
-        <v>6.6</v>
+        <v>8.9</v>
       </c>
       <c r="E24" t="n">
         <v>2.4</v>
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>Michigan -8.5</t>
+          <t>Cincinnati -5.5</t>
         </is>
       </c>
       <c r="G24" t="inlineStr">
         <is>
-          <t>Michigan -13.5</t>
+          <t>Cincinnati -5.5</t>
         </is>
       </c>
       <c r="H24" t="inlineStr">
         <is>
-          <t>Michigan -15.9</t>
+          <t>Cincinnati -7.9</t>
         </is>
       </c>
       <c r="I24" t="n">
-        <v>-15.9</v>
+        <v>7.9</v>
       </c>
       <c r="J24" t="n">
-        <v>-13.5</v>
+        <v>5.5</v>
       </c>
       <c r="K24" t="inlineStr"/>
       <c r="L24" t="inlineStr"/>
@@ -1682,7 +1682,7 @@
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>Texas Tech -36.5</t>
+          <t>Texas Tech -39.0</t>
         </is>
       </c>
       <c r="G25" t="inlineStr">
@@ -1716,40 +1716,40 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>Florida International</t>
+          <t>Navy</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>Kennesaw State</t>
+          <t>Florida Atlantic</t>
         </is>
       </c>
       <c r="D26" t="n">
-        <v>4.8</v>
+        <v>4.5</v>
       </c>
       <c r="E26" t="n">
-        <v>2.2</v>
+        <v>2.199999999999999</v>
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>Kennesaw State -1.5</t>
+          <t>Navy -14.0</t>
         </is>
       </c>
       <c r="G26" t="inlineStr">
         <is>
-          <t>Kennesaw State -1.5</t>
+          <t>Navy -15.0</t>
         </is>
       </c>
       <c r="H26" t="inlineStr">
         <is>
-          <t>Kennesaw State -3.7</t>
+          <t>Navy -17.2</t>
         </is>
       </c>
       <c r="I26" t="n">
-        <v>-3.7</v>
+        <v>17.2</v>
       </c>
       <c r="J26" t="n">
-        <v>-1.5</v>
+        <v>15</v>
       </c>
       <c r="K26" t="inlineStr"/>
       <c r="L26" t="inlineStr"/>
@@ -1766,40 +1766,40 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>Louisville</t>
+          <t>LSU</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>Boston College</t>
+          <t>Texas A&amp;M</t>
         </is>
       </c>
       <c r="D27" t="n">
-        <v>4.6</v>
+        <v>9.6</v>
       </c>
       <c r="E27" t="n">
-        <v>2.100000000000001</v>
+        <v>2.1</v>
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>Louisville -22.5</t>
+          <t>Texas A&amp;M -2.5</t>
         </is>
       </c>
       <c r="G27" t="inlineStr">
         <is>
-          <t>Louisville -23.5</t>
+          <t>Texas A&amp;M -2.5</t>
         </is>
       </c>
       <c r="H27" t="inlineStr">
         <is>
-          <t>Louisville -25.6</t>
+          <t>Texas A&amp;M -0.4</t>
         </is>
       </c>
       <c r="I27" t="n">
-        <v>25.6</v>
+        <v>-0.4</v>
       </c>
       <c r="J27" t="n">
-        <v>23.5</v>
+        <v>-2.5</v>
       </c>
       <c r="K27" t="inlineStr"/>
       <c r="L27" t="inlineStr"/>
@@ -1816,40 +1816,40 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>LSU</t>
+          <t>Kansas</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>Texas A&amp;M</t>
+          <t>Kansas State</t>
         </is>
       </c>
       <c r="D28" t="n">
-        <v>9.6</v>
+        <v>9.1</v>
       </c>
       <c r="E28" t="n">
-        <v>2.1</v>
+        <v>2</v>
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>LSU -5.5</t>
+          <t>Kansas -2.5</t>
         </is>
       </c>
       <c r="G28" t="inlineStr">
         <is>
-          <t>Texas A&amp;M -2.5</t>
+          <t>Kansas -3.0</t>
         </is>
       </c>
       <c r="H28" t="inlineStr">
         <is>
-          <t>Texas A&amp;M -0.4</t>
+          <t>Kansas -5.0</t>
         </is>
       </c>
       <c r="I28" t="n">
-        <v>-0.4</v>
+        <v>5</v>
       </c>
       <c r="J28" t="n">
-        <v>-2.5</v>
+        <v>3</v>
       </c>
       <c r="K28" t="inlineStr"/>
       <c r="L28" t="inlineStr"/>
@@ -1882,7 +1882,7 @@
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>Arizona State -7.0</t>
+          <t>Arizona State -8.5</t>
         </is>
       </c>
       <c r="G29" t="inlineStr">
@@ -1916,40 +1916,40 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>Arkansas</t>
+          <t>Michigan State</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>Auburn</t>
+          <t>Michigan</t>
         </is>
       </c>
       <c r="D30" t="n">
-        <v>9.199999999999999</v>
+        <v>6.6</v>
       </c>
       <c r="E30" t="n">
         <v>1.9</v>
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>Arkansas -1.5</t>
+          <t>Michigan -13.5</t>
         </is>
       </c>
       <c r="G30" t="inlineStr">
         <is>
-          <t>Arkansas -1.5</t>
+          <t>Michigan -14.0</t>
         </is>
       </c>
       <c r="H30" t="inlineStr">
         <is>
-          <t>Auburn -0.4</t>
+          <t>Michigan -15.9</t>
         </is>
       </c>
       <c r="I30" t="n">
-        <v>-0.4</v>
+        <v>-15.9</v>
       </c>
       <c r="J30" t="n">
-        <v>1.5</v>
+        <v>-14</v>
       </c>
       <c r="K30" t="inlineStr"/>
       <c r="L30" t="inlineStr"/>
@@ -1966,40 +1966,40 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>Arkansas State</t>
+          <t>Northern Illinois</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>Georgia Southern</t>
+          <t>Ball State</t>
         </is>
       </c>
       <c r="D31" t="n">
-        <v>5.8</v>
+        <v>4.2</v>
       </c>
       <c r="E31" t="n">
-        <v>1.9</v>
+        <v>1.8</v>
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>Arkansas State -3.0</t>
+          <t>Northern Illinois -5.0</t>
         </is>
       </c>
       <c r="G31" t="inlineStr">
         <is>
-          <t>Arkansas State -3</t>
+          <t>Northern Illinois -5.5</t>
         </is>
       </c>
       <c r="H31" t="inlineStr">
         <is>
-          <t>Arkansas State -1.1</t>
+          <t>Northern Illinois -7.3</t>
         </is>
       </c>
       <c r="I31" t="n">
-        <v>1.1</v>
+        <v>7.3</v>
       </c>
       <c r="J31" t="n">
-        <v>3</v>
+        <v>5.5</v>
       </c>
       <c r="K31" t="inlineStr"/>
       <c r="L31" t="inlineStr"/>
@@ -2016,40 +2016,40 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>Northern Illinois</t>
+          <t>Old Dominion</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>Ball State</t>
+          <t>App State</t>
         </is>
       </c>
       <c r="D32" t="n">
-        <v>4.2</v>
+        <v>5.1</v>
       </c>
       <c r="E32" t="n">
-        <v>1.8</v>
+        <v>1.5</v>
       </c>
       <c r="F32" t="inlineStr">
         <is>
-          <t>Northern Illinois -6.0</t>
+          <t>Old Dominion -13.0</t>
         </is>
       </c>
       <c r="G32" t="inlineStr">
         <is>
-          <t>Northern Illinois -5.5</t>
+          <t>Old Dominion -13.5</t>
         </is>
       </c>
       <c r="H32" t="inlineStr">
         <is>
-          <t>Northern Illinois -7.3</t>
+          <t>Old Dominion -15.0</t>
         </is>
       </c>
       <c r="I32" t="n">
-        <v>7.3</v>
+        <v>15</v>
       </c>
       <c r="J32" t="n">
-        <v>5.5</v>
+        <v>13.5</v>
       </c>
       <c r="K32" t="inlineStr"/>
       <c r="L32" t="inlineStr"/>
@@ -2066,40 +2066,40 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>Wyoming</t>
+          <t>Nevada</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>Colorado State</t>
+          <t>Boise State</t>
         </is>
       </c>
       <c r="D33" t="n">
-        <v>6.7</v>
+        <v>2.7</v>
       </c>
       <c r="E33" t="n">
-        <v>1.7</v>
+        <v>1.5</v>
       </c>
       <c r="F33" t="inlineStr">
         <is>
-          <t>Wyoming -3.5</t>
+          <t>Boise State -22.0</t>
         </is>
       </c>
       <c r="G33" t="inlineStr">
         <is>
-          <t>Wyoming -4.5</t>
+          <t>Boise State -21.5</t>
         </is>
       </c>
       <c r="H33" t="inlineStr">
         <is>
-          <t>Wyoming -2.8</t>
+          <t>Boise State -23.0</t>
         </is>
       </c>
       <c r="I33" t="n">
-        <v>2.8</v>
+        <v>-23</v>
       </c>
       <c r="J33" t="n">
-        <v>4.5</v>
+        <v>-21.5</v>
       </c>
       <c r="K33" t="inlineStr"/>
       <c r="L33" t="inlineStr"/>
@@ -2116,40 +2116,40 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>Georgia Tech</t>
+          <t>Eastern Michigan</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>Syracuse</t>
+          <t>Ohio</t>
         </is>
       </c>
       <c r="D34" t="n">
-        <v>6.9</v>
+        <v>3.7</v>
       </c>
       <c r="E34" t="n">
-        <v>1.5</v>
+        <v>1.4</v>
       </c>
       <c r="F34" t="inlineStr">
         <is>
-          <t>Georgia Tech -18.5</t>
+          <t>Ohio -10.5</t>
         </is>
       </c>
       <c r="G34" t="inlineStr">
         <is>
-          <t>Georgia Tech -18.5</t>
+          <t>Ohio -12.5</t>
         </is>
       </c>
       <c r="H34" t="inlineStr">
         <is>
-          <t>Georgia Tech -17.0</t>
+          <t>Ohio -11.1</t>
         </is>
       </c>
       <c r="I34" t="n">
-        <v>17</v>
+        <v>-11.1</v>
       </c>
       <c r="J34" t="n">
-        <v>18.5</v>
+        <v>-12.5</v>
       </c>
       <c r="K34" t="inlineStr"/>
       <c r="L34" t="inlineStr"/>
@@ -2166,40 +2166,40 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>Troy</t>
+          <t>Kent State</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>Louisiana</t>
+          <t>Bowling Green</t>
         </is>
       </c>
       <c r="D35" t="n">
-        <v>5.3</v>
+        <v>2.8</v>
       </c>
       <c r="E35" t="n">
-        <v>1.5</v>
+        <v>1.300000000000001</v>
       </c>
       <c r="F35" t="inlineStr">
         <is>
-          <t>Troy -8.5</t>
+          <t>Bowling Green -8.5</t>
         </is>
       </c>
       <c r="G35" t="inlineStr">
         <is>
-          <t>Troy -9.5</t>
+          <t>Bowling Green -8.5</t>
         </is>
       </c>
       <c r="H35" t="inlineStr">
         <is>
-          <t>Troy -11.0</t>
+          <t>Bowling Green -9.8</t>
         </is>
       </c>
       <c r="I35" t="n">
-        <v>11</v>
+        <v>-9.800000000000001</v>
       </c>
       <c r="J35" t="n">
-        <v>9.5</v>
+        <v>-8.5</v>
       </c>
       <c r="K35" t="inlineStr"/>
       <c r="L35" t="inlineStr"/>
@@ -2216,40 +2216,40 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>Old Dominion</t>
+          <t>Vanderbilt</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>App State</t>
+          <t>Missouri</t>
         </is>
       </c>
       <c r="D36" t="n">
-        <v>5.1</v>
+        <v>9.699999999999999</v>
       </c>
       <c r="E36" t="n">
-        <v>1.5</v>
+        <v>1.2</v>
       </c>
       <c r="F36" t="inlineStr">
         <is>
-          <t>Old Dominion -13.5</t>
+          <t>Vanderbilt -3.0</t>
         </is>
       </c>
       <c r="G36" t="inlineStr">
         <is>
-          <t>Old Dominion -13.5</t>
+          <t>Vanderbilt -3.0</t>
         </is>
       </c>
       <c r="H36" t="inlineStr">
         <is>
-          <t>Old Dominion -15.0</t>
+          <t>Vanderbilt -1.8</t>
         </is>
       </c>
       <c r="I36" t="n">
-        <v>15</v>
+        <v>1.8</v>
       </c>
       <c r="J36" t="n">
-        <v>13.5</v>
+        <v>3</v>
       </c>
       <c r="K36" t="inlineStr"/>
       <c r="L36" t="inlineStr"/>
@@ -2266,40 +2266,40 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>Pittsburgh</t>
+          <t>Charlotte</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>NC State</t>
+          <t>North Texas</t>
         </is>
       </c>
       <c r="D37" t="n">
-        <v>8.4</v>
+        <v>1.9</v>
       </c>
       <c r="E37" t="n">
-        <v>1.4</v>
+        <v>1.100000000000001</v>
       </c>
       <c r="F37" t="inlineStr">
         <is>
-          <t>Pittsburgh -7.5</t>
+          <t>North Texas -27.0</t>
         </is>
       </c>
       <c r="G37" t="inlineStr">
         <is>
-          <t>Pittsburgh -8.5</t>
+          <t>North Texas -27.0</t>
         </is>
       </c>
       <c r="H37" t="inlineStr">
         <is>
-          <t>Pittsburgh -9.9</t>
+          <t>North Texas -28.1</t>
         </is>
       </c>
       <c r="I37" t="n">
-        <v>9.9</v>
+        <v>-28.1</v>
       </c>
       <c r="J37" t="n">
-        <v>8.5</v>
+        <v>-27</v>
       </c>
       <c r="K37" t="inlineStr"/>
       <c r="L37" t="inlineStr"/>
@@ -2316,40 +2316,40 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>Kent State</t>
+          <t>Arkansas</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>Bowling Green</t>
+          <t>Auburn</t>
         </is>
       </c>
       <c r="D38" t="n">
-        <v>2.8</v>
+        <v>9.199999999999999</v>
       </c>
       <c r="E38" t="n">
-        <v>1.300000000000001</v>
+        <v>1.1</v>
       </c>
       <c r="F38" t="inlineStr">
         <is>
-          <t>Bowling Green -10.0</t>
+          <t>Arkansas --0.0</t>
         </is>
       </c>
       <c r="G38" t="inlineStr">
         <is>
-          <t>Bowling Green -8.5</t>
+          <t>Auburn -1.5</t>
         </is>
       </c>
       <c r="H38" t="inlineStr">
         <is>
-          <t>Bowling Green -9.8</t>
+          <t>Auburn -0.4</t>
         </is>
       </c>
       <c r="I38" t="n">
-        <v>-9.800000000000001</v>
+        <v>-0.4</v>
       </c>
       <c r="J38" t="n">
-        <v>-8.5</v>
+        <v>-1.5</v>
       </c>
       <c r="K38" t="inlineStr"/>
       <c r="L38" t="inlineStr"/>
@@ -2366,40 +2366,40 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>Fresno State</t>
+          <t>West Virginia</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>San Diego State</t>
+          <t>TCU</t>
         </is>
       </c>
       <c r="D39" t="n">
-        <v>6.9</v>
+        <v>5.8</v>
       </c>
       <c r="E39" t="n">
-        <v>1.2</v>
+        <v>0.9000000000000004</v>
       </c>
       <c r="F39" t="inlineStr">
         <is>
-          <t>San Diego State -2.5</t>
+          <t>TCU -15.0</t>
         </is>
       </c>
       <c r="G39" t="inlineStr">
         <is>
-          <t>San Diego State -2.5</t>
+          <t>TCU -15.0</t>
         </is>
       </c>
       <c r="H39" t="inlineStr">
         <is>
-          <t>San Diego State -3.7</t>
+          <t>TCU -14.1</t>
         </is>
       </c>
       <c r="I39" t="n">
-        <v>-3.7</v>
+        <v>-14.1</v>
       </c>
       <c r="J39" t="n">
-        <v>-2.5</v>
+        <v>-15</v>
       </c>
       <c r="K39" t="inlineStr"/>
       <c r="L39" t="inlineStr"/>
@@ -2416,40 +2416,40 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>Eastern Michigan</t>
+          <t>Washington</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>Ohio</t>
+          <t>Illinois</t>
         </is>
       </c>
       <c r="D40" t="n">
-        <v>3.7</v>
+        <v>9.5</v>
       </c>
       <c r="E40" t="n">
-        <v>1.1</v>
+        <v>0.8999999999999999</v>
       </c>
       <c r="F40" t="inlineStr">
         <is>
-          <t>Ohio -10.0</t>
+          <t>Washington -5.0</t>
         </is>
       </c>
       <c r="G40" t="inlineStr">
         <is>
-          <t>Ohio -10</t>
+          <t>Washington -4.5</t>
         </is>
       </c>
       <c r="H40" t="inlineStr">
         <is>
-          <t>Ohio -11.1</t>
+          <t>Washington -3.6</t>
         </is>
       </c>
       <c r="I40" t="n">
-        <v>-11.1</v>
+        <v>3.6</v>
       </c>
       <c r="J40" t="n">
-        <v>-10</v>
+        <v>4.5</v>
       </c>
       <c r="K40" t="inlineStr"/>
       <c r="L40" t="inlineStr"/>
@@ -2466,40 +2466,40 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>Purdue</t>
+          <t>Arkansas State</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>Rutgers</t>
+          <t>Georgia Southern</t>
         </is>
       </c>
       <c r="D41" t="n">
-        <v>7.7</v>
+        <v>5.8</v>
       </c>
       <c r="E41" t="n">
-        <v>0.8</v>
+        <v>0.8999999999999999</v>
       </c>
       <c r="F41" t="inlineStr">
         <is>
-          <t>Rutgers -2.5</t>
+          <t>Arkansas State -2.0</t>
         </is>
       </c>
       <c r="G41" t="inlineStr">
         <is>
-          <t>Rutgers -2.5</t>
+          <t>Arkansas State -2.0</t>
         </is>
       </c>
       <c r="H41" t="inlineStr">
         <is>
-          <t>Rutgers -1.7</t>
+          <t>Arkansas State -1.1</t>
         </is>
       </c>
       <c r="I41" t="n">
-        <v>-1.7</v>
+        <v>1.1</v>
       </c>
       <c r="J41" t="n">
-        <v>-2.5</v>
+        <v>2</v>
       </c>
       <c r="K41" t="inlineStr"/>
       <c r="L41" t="inlineStr"/>
@@ -2516,40 +2516,40 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>Georgia State</t>
+          <t>Purdue</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>South Alabama</t>
+          <t>Rutgers</t>
         </is>
       </c>
       <c r="D42" t="n">
-        <v>3.5</v>
+        <v>7.7</v>
       </c>
       <c r="E42" t="n">
-        <v>0.7000000000000002</v>
+        <v>0.8</v>
       </c>
       <c r="F42" t="inlineStr">
         <is>
-          <t>South Alabama -6.5</t>
+          <t>Rutgers -2.5</t>
         </is>
       </c>
       <c r="G42" t="inlineStr">
         <is>
-          <t>South Alabama -6.5</t>
+          <t>Rutgers -2.5</t>
         </is>
       </c>
       <c r="H42" t="inlineStr">
         <is>
-          <t>South Alabama -7.2</t>
+          <t>Rutgers -1.7</t>
         </is>
       </c>
       <c r="I42" t="n">
-        <v>-7.2</v>
+        <v>-1.7</v>
       </c>
       <c r="J42" t="n">
-        <v>-6.5</v>
+        <v>-2.5</v>
       </c>
       <c r="K42" t="inlineStr"/>
       <c r="L42" t="inlineStr"/>
@@ -2566,40 +2566,40 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>Vanderbilt</t>
+          <t>Florida International</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>Missouri</t>
+          <t>Kennesaw State</t>
         </is>
       </c>
       <c r="D43" t="n">
-        <v>9.699999999999999</v>
+        <v>4.8</v>
       </c>
       <c r="E43" t="n">
-        <v>0.7</v>
+        <v>0.7000000000000002</v>
       </c>
       <c r="F43" t="inlineStr">
         <is>
-          <t>Vanderbilt -1.5</t>
+          <t>Kennesaw State -1.5</t>
         </is>
       </c>
       <c r="G43" t="inlineStr">
         <is>
-          <t>Vanderbilt -2.5</t>
+          <t>Kennesaw State -3.0</t>
         </is>
       </c>
       <c r="H43" t="inlineStr">
         <is>
-          <t>Vanderbilt -1.8</t>
+          <t>Kennesaw State -3.7</t>
         </is>
       </c>
       <c r="I43" t="n">
-        <v>1.8</v>
+        <v>-3.7</v>
       </c>
       <c r="J43" t="n">
-        <v>2.5</v>
+        <v>-3</v>
       </c>
       <c r="K43" t="inlineStr"/>
       <c r="L43" t="inlineStr"/>
@@ -2616,40 +2616,40 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>South Carolina</t>
+          <t>Georgia State</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>Alabama</t>
+          <t>South Alabama</t>
         </is>
       </c>
       <c r="D44" t="n">
-        <v>8.4</v>
+        <v>3.5</v>
       </c>
       <c r="E44" t="n">
-        <v>0.6999999999999993</v>
+        <v>0.7000000000000002</v>
       </c>
       <c r="F44" t="inlineStr">
         <is>
-          <t>Alabama -7.5</t>
+          <t>South Alabama -6.0</t>
         </is>
       </c>
       <c r="G44" t="inlineStr">
         <is>
-          <t>Alabama -13.5</t>
+          <t>South Alabama -6.5</t>
         </is>
       </c>
       <c r="H44" t="inlineStr">
         <is>
-          <t>Alabama -12.8</t>
+          <t>South Alabama -7.2</t>
         </is>
       </c>
       <c r="I44" t="n">
-        <v>-12.8</v>
+        <v>-7.2</v>
       </c>
       <c r="J44" t="n">
-        <v>-13.5</v>
+        <v>-6.5</v>
       </c>
       <c r="K44" t="inlineStr"/>
       <c r="L44" t="inlineStr"/>
@@ -2666,40 +2666,40 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>Charlotte</t>
+          <t>Louisville</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>North Texas</t>
+          <t>Boston College</t>
         </is>
       </c>
       <c r="D45" t="n">
-        <v>1.9</v>
+        <v>4.6</v>
       </c>
       <c r="E45" t="n">
         <v>0.6000000000000014</v>
       </c>
       <c r="F45" t="inlineStr">
         <is>
-          <t>North Texas -27.5</t>
+          <t>Louisville -24.5</t>
         </is>
       </c>
       <c r="G45" t="inlineStr">
         <is>
-          <t>North Texas -27.5</t>
+          <t>Louisville -25.0</t>
         </is>
       </c>
       <c r="H45" t="inlineStr">
         <is>
-          <t>North Texas -28.1</t>
+          <t>Louisville -25.6</t>
         </is>
       </c>
       <c r="I45" t="n">
-        <v>-28.1</v>
+        <v>25.6</v>
       </c>
       <c r="J45" t="n">
-        <v>-27.5</v>
+        <v>25</v>
       </c>
       <c r="K45" t="inlineStr"/>
       <c r="L45" t="inlineStr"/>
@@ -2716,40 +2716,40 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>Virginia Tech</t>
+          <t>Miami</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>California</t>
+          <t>Stanford</t>
         </is>
       </c>
       <c r="D46" t="n">
-        <v>7.8</v>
+        <v>4.5</v>
       </c>
       <c r="E46" t="n">
         <v>0.5</v>
       </c>
       <c r="F46" t="inlineStr">
         <is>
-          <t>Virginia Tech -2.5</t>
+          <t>Miami -30.0</t>
         </is>
       </c>
       <c r="G46" t="inlineStr">
         <is>
-          <t>Virginia Tech -4</t>
+          <t>Miami -30.0</t>
         </is>
       </c>
       <c r="H46" t="inlineStr">
         <is>
-          <t>Virginia Tech -3.5</t>
+          <t>Miami -30.5</t>
         </is>
       </c>
       <c r="I46" t="n">
-        <v>3.5</v>
+        <v>30.5</v>
       </c>
       <c r="J46" t="n">
-        <v>4</v>
+        <v>30</v>
       </c>
       <c r="K46" t="inlineStr"/>
       <c r="L46" t="inlineStr"/>
@@ -2766,40 +2766,40 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>Nevada</t>
+          <t>Georgia Tech</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>Boise State</t>
+          <t>Syracuse</t>
         </is>
       </c>
       <c r="D47" t="n">
-        <v>2.7</v>
+        <v>6.9</v>
       </c>
       <c r="E47" t="n">
         <v>0.5</v>
       </c>
       <c r="F47" t="inlineStr">
         <is>
-          <t>Boise State -21.5</t>
+          <t>Georgia Tech -18.0</t>
         </is>
       </c>
       <c r="G47" t="inlineStr">
         <is>
-          <t>Boise State -22.5</t>
+          <t>Georgia Tech -17.5</t>
         </is>
       </c>
       <c r="H47" t="inlineStr">
         <is>
-          <t>Boise State -23.0</t>
+          <t>Georgia Tech -17.0</t>
         </is>
       </c>
       <c r="I47" t="n">
-        <v>-23</v>
+        <v>17</v>
       </c>
       <c r="J47" t="n">
-        <v>-22.5</v>
+        <v>17.5</v>
       </c>
       <c r="K47" t="inlineStr"/>
       <c r="L47" t="inlineStr"/>
@@ -2816,40 +2816,40 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>Kentucky</t>
+          <t>Virginia Tech</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>Tennessee</t>
+          <t>California</t>
         </is>
       </c>
       <c r="D48" t="n">
-        <v>8.199999999999999</v>
+        <v>7.8</v>
       </c>
       <c r="E48" t="n">
-        <v>0.4000000000000004</v>
+        <v>0.5</v>
       </c>
       <c r="F48" t="inlineStr">
         <is>
-          <t>Tennessee -9.5</t>
+          <t>Virginia Tech -4.5</t>
         </is>
       </c>
       <c r="G48" t="inlineStr">
         <is>
-          <t>Tennessee -9.5</t>
+          <t>Virginia Tech -4.0</t>
         </is>
       </c>
       <c r="H48" t="inlineStr">
         <is>
-          <t>Tennessee -9.1</t>
+          <t>Virginia Tech -3.5</t>
         </is>
       </c>
       <c r="I48" t="n">
-        <v>-9.1</v>
+        <v>3.5</v>
       </c>
       <c r="J48" t="n">
-        <v>-9.5</v>
+        <v>4</v>
       </c>
       <c r="K48" t="inlineStr"/>
       <c r="L48" t="inlineStr"/>
@@ -2866,40 +2866,40 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>West Virginia</t>
+          <t>Kentucky</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>TCU</t>
+          <t>Tennessee</t>
         </is>
       </c>
       <c r="D49" t="n">
-        <v>5.8</v>
+        <v>8.199999999999999</v>
       </c>
       <c r="E49" t="n">
         <v>0.4000000000000004</v>
       </c>
       <c r="F49" t="inlineStr">
         <is>
-          <t>TCU -14.5</t>
+          <t>Tennessee -9.0</t>
         </is>
       </c>
       <c r="G49" t="inlineStr">
         <is>
-          <t>TCU -14.5</t>
+          <t>Tennessee -9.5</t>
         </is>
       </c>
       <c r="H49" t="inlineStr">
         <is>
-          <t>TCU -14.1</t>
+          <t>Tennessee -9.1</t>
         </is>
       </c>
       <c r="I49" t="n">
-        <v>-14.1</v>
+        <v>-9.1</v>
       </c>
       <c r="J49" t="n">
-        <v>-14.5</v>
+        <v>-9.5</v>
       </c>
       <c r="K49" t="inlineStr"/>
       <c r="L49" t="inlineStr"/>
@@ -2916,40 +2916,40 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>Washington</t>
+          <t>New Mexico</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>Illinois</t>
+          <t>Utah State</t>
         </is>
       </c>
       <c r="D50" t="n">
-        <v>9.5</v>
+        <v>7.5</v>
       </c>
       <c r="E50" t="n">
         <v>0.3999999999999999</v>
       </c>
       <c r="F50" t="inlineStr">
         <is>
-          <t>Washington -4.5</t>
+          <t>New Mexico -2.5</t>
         </is>
       </c>
       <c r="G50" t="inlineStr">
         <is>
-          <t>Washington -4</t>
+          <t>New Mexico -2.5</t>
         </is>
       </c>
       <c r="H50" t="inlineStr">
         <is>
-          <t>Washington -3.6</t>
+          <t>New Mexico -2.9</t>
         </is>
       </c>
       <c r="I50" t="n">
-        <v>3.6</v>
+        <v>2.9</v>
       </c>
       <c r="J50" t="n">
-        <v>4</v>
+        <v>2.5</v>
       </c>
       <c r="K50" t="inlineStr"/>
       <c r="L50" t="inlineStr"/>
@@ -2966,40 +2966,40 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>New Mexico</t>
+          <t>Oklahoma</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>Utah State</t>
+          <t>Ole Miss</t>
         </is>
       </c>
       <c r="D51" t="n">
-        <v>7.5</v>
+        <v>9.699999999999999</v>
       </c>
       <c r="E51" t="n">
-        <v>0.3999999999999999</v>
+        <v>0.2999999999999998</v>
       </c>
       <c r="F51" t="inlineStr">
         <is>
-          <t>New Mexico -1.5</t>
+          <t>Oklahoma -4.5</t>
         </is>
       </c>
       <c r="G51" t="inlineStr">
         <is>
-          <t>New Mexico -2.5</t>
+          <t>Oklahoma -4.0</t>
         </is>
       </c>
       <c r="H51" t="inlineStr">
         <is>
-          <t>New Mexico -2.9</t>
+          <t>Oklahoma -4.3</t>
         </is>
       </c>
       <c r="I51" t="n">
-        <v>2.9</v>
+        <v>4.3</v>
       </c>
       <c r="J51" t="n">
-        <v>2.5</v>
+        <v>4</v>
       </c>
       <c r="K51" t="inlineStr"/>
       <c r="L51" t="inlineStr"/>
@@ -3016,40 +3016,40 @@
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>Oklahoma</t>
+          <t>Fresno State</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>Ole Miss</t>
+          <t>San Diego State</t>
         </is>
       </c>
       <c r="D52" t="n">
-        <v>9.699999999999999</v>
+        <v>6.9</v>
       </c>
       <c r="E52" t="n">
-        <v>0.2999999999999998</v>
+        <v>0.2000000000000002</v>
       </c>
       <c r="F52" t="inlineStr">
         <is>
-          <t>Oklahoma -2.5</t>
+          <t>San Diego State -2.5</t>
         </is>
       </c>
       <c r="G52" t="inlineStr">
         <is>
-          <t>Oklahoma -4</t>
+          <t>San Diego State -3.5</t>
         </is>
       </c>
       <c r="H52" t="inlineStr">
         <is>
-          <t>Oklahoma -4.3</t>
+          <t>San Diego State -3.7</t>
         </is>
       </c>
       <c r="I52" t="n">
-        <v>4.3</v>
+        <v>-3.7</v>
       </c>
       <c r="J52" t="n">
-        <v>4</v>
+        <v>-3.5</v>
       </c>
       <c r="K52" t="inlineStr"/>
       <c r="L52" t="inlineStr"/>
@@ -3066,40 +3066,40 @@
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>Miami (OH)</t>
+          <t>South Carolina</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>Western Michigan</t>
+          <t>Alabama</t>
         </is>
       </c>
       <c r="D53" t="n">
-        <v>7.1</v>
+        <v>8.4</v>
       </c>
       <c r="E53" t="n">
-        <v>0.1000000000000001</v>
+        <v>0.1999999999999993</v>
       </c>
       <c r="F53" t="inlineStr">
         <is>
-          <t>Miami (OH) -3.5</t>
+          <t>Alabama -13.0</t>
         </is>
       </c>
       <c r="G53" t="inlineStr">
         <is>
-          <t>Miami (OH) -2.5</t>
+          <t>Alabama -13.0</t>
         </is>
       </c>
       <c r="H53" t="inlineStr">
         <is>
-          <t>Miami (OH) -2.4</t>
+          <t>Alabama -12.8</t>
         </is>
       </c>
       <c r="I53" t="n">
-        <v>2.4</v>
+        <v>-12.8</v>
       </c>
       <c r="J53" t="n">
-        <v>2.5</v>
+        <v>-13</v>
       </c>
       <c r="K53" t="inlineStr"/>
       <c r="L53" t="inlineStr"/>
@@ -3116,40 +3116,40 @@
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>Miami</t>
+          <t>Miami (OH)</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>Stanford</t>
+          <t>Western Michigan</t>
         </is>
       </c>
       <c r="D54" t="n">
-        <v>4.5</v>
+        <v>7.1</v>
       </c>
       <c r="E54" t="n">
-        <v>0</v>
+        <v>0.1000000000000001</v>
       </c>
       <c r="F54" t="inlineStr">
         <is>
-          <t>Miami -30.5</t>
+          <t>Miami (OH) -2.0</t>
         </is>
       </c>
       <c r="G54" t="inlineStr">
         <is>
-          <t>Miami -30.5</t>
+          <t>Miami (OH) -2.5</t>
         </is>
       </c>
       <c r="H54" t="inlineStr">
         <is>
-          <t>Miami -30.5</t>
+          <t>Miami (OH) -2.4</t>
         </is>
       </c>
       <c r="I54" t="n">
-        <v>30.5</v>
+        <v>2.4</v>
       </c>
       <c r="J54" t="n">
-        <v>30.5</v>
+        <v>2.5</v>
       </c>
       <c r="K54" t="inlineStr"/>
       <c r="L54" t="inlineStr"/>

</xml_diff>

<commit_message>
Creating the offense versus defense PPA and Success rate graphs
</commit_message>
<xml_diff>
--- a/PEAR/PEAR Football/y2025/Spreads/spreads_tracker_week9.xlsx
+++ b/PEAR/PEAR Football/y2025/Spreads/spreads_tracker_week9.xlsx
@@ -516,40 +516,40 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Delaware</t>
+          <t>Washington State</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Middle Tennessee</t>
+          <t>Toledo</t>
         </is>
       </c>
       <c r="D2" t="n">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="E2" t="n">
-        <v>6.9</v>
+        <v>7.1</v>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>Delaware -10.0</t>
+          <t>Washington State -1.5</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>Delaware -8.5</t>
+          <t>Washington State -2.0</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>Delaware -15.4</t>
+          <t>Toledo -5.1</t>
         </is>
       </c>
       <c r="I2" t="n">
-        <v>15.4</v>
+        <v>-5.1</v>
       </c>
       <c r="J2" t="n">
-        <v>8.5</v>
+        <v>2</v>
       </c>
       <c r="K2" t="inlineStr"/>
       <c r="L2" t="inlineStr"/>
@@ -566,40 +566,40 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Memphis</t>
+          <t>Delaware</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>South Florida</t>
+          <t>Middle Tennessee</t>
         </is>
       </c>
       <c r="D3" t="n">
-        <v>9.300000000000001</v>
+        <v>3</v>
       </c>
       <c r="E3" t="n">
         <v>6.9</v>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>South Florida -3.5</t>
+          <t>Delaware -10.0</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>South Florida -4.0</t>
+          <t>Delaware -8.5</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>Memphis -2.9</t>
+          <t>Delaware -15.4</t>
         </is>
       </c>
       <c r="I3" t="n">
-        <v>2.9</v>
+        <v>15.4</v>
       </c>
       <c r="J3" t="n">
-        <v>-4</v>
+        <v>8.5</v>
       </c>
       <c r="K3" t="inlineStr"/>
       <c r="L3" t="inlineStr"/>
@@ -616,40 +616,40 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Washington State</t>
+          <t>Memphis</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Toledo</t>
+          <t>South Florida</t>
         </is>
       </c>
       <c r="D4" t="n">
-        <v>7</v>
+        <v>9.300000000000001</v>
       </c>
       <c r="E4" t="n">
-        <v>6.6</v>
+        <v>6.9</v>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>Washington State -1.5</t>
+          <t>South Florida -3.5</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>Washington State -1.5</t>
+          <t>South Florida -4.0</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>Toledo -5.1</t>
+          <t>Memphis -2.9</t>
         </is>
       </c>
       <c r="I4" t="n">
-        <v>-5.1</v>
+        <v>2.9</v>
       </c>
       <c r="J4" t="n">
-        <v>1.5</v>
+        <v>-4</v>
       </c>
       <c r="K4" t="inlineStr"/>
       <c r="L4" t="inlineStr"/>
@@ -678,7 +678,7 @@
         <v>3.1</v>
       </c>
       <c r="E5" t="n">
-        <v>6.5</v>
+        <v>6</v>
       </c>
       <c r="F5" t="inlineStr">
         <is>
@@ -687,7 +687,7 @@
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>Buffalo -9.0</t>
+          <t>Buffalo -9.5</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
@@ -699,7 +699,7 @@
         <v>15.5</v>
       </c>
       <c r="J5" t="n">
-        <v>9</v>
+        <v>9.5</v>
       </c>
       <c r="K5" t="inlineStr"/>
       <c r="L5" t="inlineStr"/>
@@ -728,7 +728,7 @@
         <v>8.199999999999999</v>
       </c>
       <c r="E6" t="n">
-        <v>5.6</v>
+        <v>5.1</v>
       </c>
       <c r="F6" t="inlineStr">
         <is>
@@ -737,7 +737,7 @@
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>Nebraska -6.5</t>
+          <t>Nebraska -7.0</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
@@ -749,7 +749,7 @@
         <v>12.1</v>
       </c>
       <c r="J6" t="n">
-        <v>6.5</v>
+        <v>7</v>
       </c>
       <c r="K6" t="inlineStr"/>
       <c r="L6" t="inlineStr"/>
@@ -766,40 +766,40 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Indiana</t>
+          <t>Iowa State</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>UCLA</t>
+          <t>BYU</t>
         </is>
       </c>
       <c r="D7" t="n">
-        <v>6.1</v>
+        <v>9.199999999999999</v>
       </c>
       <c r="E7" t="n">
-        <v>5.300000000000001</v>
+        <v>4.8</v>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>Indiana -24.5</t>
+          <t>Iowa State -2.0</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>Indiana -24.0</t>
+          <t>Iowa State -2.5</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>Indiana -29.3</t>
+          <t>BYU -2.3</t>
         </is>
       </c>
       <c r="I7" t="n">
-        <v>29.3</v>
+        <v>-2.3</v>
       </c>
       <c r="J7" t="n">
-        <v>24</v>
+        <v>2.5</v>
       </c>
       <c r="K7" t="inlineStr"/>
       <c r="L7" t="inlineStr"/>
@@ -816,40 +816,40 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Iowa State</t>
+          <t>Indiana</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>BYU</t>
+          <t>UCLA</t>
         </is>
       </c>
       <c r="D8" t="n">
-        <v>9.199999999999999</v>
+        <v>6.1</v>
       </c>
       <c r="E8" t="n">
-        <v>4.8</v>
+        <v>4.300000000000001</v>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>Iowa State -2.0</t>
+          <t>Indiana -24.5</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>Iowa State -2.5</t>
+          <t>Indiana -25.0</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>BYU -2.3</t>
+          <t>Indiana -29.3</t>
         </is>
       </c>
       <c r="I8" t="n">
-        <v>-2.3</v>
+        <v>29.3</v>
       </c>
       <c r="J8" t="n">
-        <v>2.5</v>
+        <v>25</v>
       </c>
       <c r="K8" t="inlineStr"/>
       <c r="L8" t="inlineStr"/>
@@ -916,40 +916,40 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Iowa</t>
+          <t>Rice</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Minnesota</t>
+          <t>UConn</t>
         </is>
       </c>
       <c r="D10" t="n">
-        <v>8.5</v>
+        <v>3.7</v>
       </c>
       <c r="E10" t="n">
-        <v>3.9</v>
+        <v>4.300000000000001</v>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>Iowa -7.5</t>
+          <t>UConn -10.0</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>Iowa -8.5</t>
+          <t>UConn -10.0</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>Iowa -12.4</t>
+          <t>UConn -14.3</t>
         </is>
       </c>
       <c r="I10" t="n">
-        <v>12.4</v>
+        <v>-14.3</v>
       </c>
       <c r="J10" t="n">
-        <v>8.5</v>
+        <v>-10</v>
       </c>
       <c r="K10" t="inlineStr"/>
       <c r="L10" t="inlineStr"/>
@@ -966,40 +966,40 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>North Carolina</t>
+          <t>Utah</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Virginia</t>
+          <t>Colorado</t>
         </is>
       </c>
       <c r="D11" t="n">
-        <v>5.2</v>
+        <v>7.8</v>
       </c>
       <c r="E11" t="n">
-        <v>3.9</v>
+        <v>4</v>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>Virginia -9.0</t>
+          <t>Utah -15.5</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>Virginia -10.0</t>
+          <t>Utah -14.0</t>
         </is>
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>Virginia -13.9</t>
+          <t>Utah -18.0</t>
         </is>
       </c>
       <c r="I11" t="n">
-        <v>-13.9</v>
+        <v>18</v>
       </c>
       <c r="J11" t="n">
-        <v>-10</v>
+        <v>14</v>
       </c>
       <c r="K11" t="inlineStr"/>
       <c r="L11" t="inlineStr"/>
@@ -1016,40 +1016,40 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Rice</t>
+          <t>Iowa</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>UConn</t>
+          <t>Minnesota</t>
         </is>
       </c>
       <c r="D12" t="n">
-        <v>3.7</v>
+        <v>8.5</v>
       </c>
       <c r="E12" t="n">
-        <v>3.800000000000001</v>
+        <v>3.9</v>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>UConn -10.0</t>
+          <t>Iowa -7.5</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>UConn -10.5</t>
+          <t>Iowa -8.5</t>
         </is>
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>UConn -14.3</t>
+          <t>Iowa -12.4</t>
         </is>
       </c>
       <c r="I12" t="n">
-        <v>-14.3</v>
+        <v>12.4</v>
       </c>
       <c r="J12" t="n">
-        <v>-10.5</v>
+        <v>8.5</v>
       </c>
       <c r="K12" t="inlineStr"/>
       <c r="L12" t="inlineStr"/>
@@ -1216,40 +1216,40 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Wyoming</t>
+          <t>Pittsburgh</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>Colorado State</t>
+          <t>NC State</t>
         </is>
       </c>
       <c r="D16" t="n">
-        <v>6.7</v>
+        <v>8.4</v>
       </c>
       <c r="E16" t="n">
-        <v>3.2</v>
+        <v>3.4</v>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>Wyoming -5.0</t>
+          <t>Pittsburgh -8.5</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>Wyoming -6.0</t>
+          <t>Pittsburgh -6.5</t>
         </is>
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>Wyoming -2.8</t>
+          <t>Pittsburgh -9.9</t>
         </is>
       </c>
       <c r="I16" t="n">
-        <v>2.8</v>
+        <v>9.9</v>
       </c>
       <c r="J16" t="n">
-        <v>6</v>
+        <v>6.5</v>
       </c>
       <c r="K16" t="inlineStr"/>
       <c r="L16" t="inlineStr"/>
@@ -1266,40 +1266,40 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Oregon</t>
+          <t>Cincinnati</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>Wisconsin</t>
+          <t>Baylor</t>
         </is>
       </c>
       <c r="D17" t="n">
-        <v>5.5</v>
+        <v>8.9</v>
       </c>
       <c r="E17" t="n">
-        <v>3.199999999999999</v>
+        <v>3.4</v>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>Oregon -34.0</t>
+          <t>Cincinnati -5.5</t>
         </is>
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>Oregon -34.5</t>
+          <t>Cincinnati -4.5</t>
         </is>
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t>Oregon -31.3</t>
+          <t>Cincinnati -7.9</t>
         </is>
       </c>
       <c r="I17" t="n">
-        <v>31.3</v>
+        <v>7.9</v>
       </c>
       <c r="J17" t="n">
-        <v>34.5</v>
+        <v>4.5</v>
       </c>
       <c r="K17" t="inlineStr"/>
       <c r="L17" t="inlineStr"/>
@@ -1316,40 +1316,40 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Mississippi State</t>
+          <t>North Carolina</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>Texas</t>
+          <t>Virginia</t>
         </is>
       </c>
       <c r="D18" t="n">
-        <v>8.699999999999999</v>
+        <v>5.2</v>
       </c>
       <c r="E18" t="n">
-        <v>3.1</v>
+        <v>3.4</v>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>Texas -6.5</t>
+          <t>Virginia -9.0</t>
         </is>
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>Texas -6.5</t>
+          <t>Virginia -10.5</t>
         </is>
       </c>
       <c r="H18" t="inlineStr">
         <is>
-          <t>Texas -9.6</t>
+          <t>Virginia -13.9</t>
         </is>
       </c>
       <c r="I18" t="n">
-        <v>-9.6</v>
+        <v>-13.9</v>
       </c>
       <c r="J18" t="n">
-        <v>-6.5</v>
+        <v>-10.5</v>
       </c>
       <c r="K18" t="inlineStr"/>
       <c r="L18" t="inlineStr"/>
@@ -1366,40 +1366,40 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Utah</t>
+          <t>Wyoming</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>Colorado</t>
+          <t>Colorado State</t>
         </is>
       </c>
       <c r="D19" t="n">
-        <v>7.8</v>
+        <v>6.7</v>
       </c>
       <c r="E19" t="n">
-        <v>3</v>
+        <v>3.2</v>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>Utah -15.5</t>
+          <t>Wyoming -5.0</t>
         </is>
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>Utah -15.0</t>
+          <t>Wyoming -6.0</t>
         </is>
       </c>
       <c r="H19" t="inlineStr">
         <is>
-          <t>Utah -18.0</t>
+          <t>Wyoming -2.8</t>
         </is>
       </c>
       <c r="I19" t="n">
-        <v>18</v>
+        <v>2.8</v>
       </c>
       <c r="J19" t="n">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="K19" t="inlineStr"/>
       <c r="L19" t="inlineStr"/>
@@ -1416,40 +1416,40 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Wake Forest</t>
+          <t>Oregon</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>SMU</t>
+          <t>Wisconsin</t>
         </is>
       </c>
       <c r="D20" t="n">
-        <v>7.8</v>
+        <v>5.5</v>
       </c>
       <c r="E20" t="n">
-        <v>3</v>
+        <v>3.199999999999999</v>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>SMU -3.5</t>
+          <t>Oregon -34.0</t>
         </is>
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>SMU -3.5</t>
+          <t>Oregon -34.5</t>
         </is>
       </c>
       <c r="H20" t="inlineStr">
         <is>
-          <t>SMU -6.5</t>
+          <t>Oregon -31.3</t>
         </is>
       </c>
       <c r="I20" t="n">
-        <v>-6.5</v>
+        <v>31.3</v>
       </c>
       <c r="J20" t="n">
-        <v>-3.5</v>
+        <v>34.5</v>
       </c>
       <c r="K20" t="inlineStr"/>
       <c r="L20" t="inlineStr"/>
@@ -1466,40 +1466,40 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Pittsburgh</t>
+          <t>Mississippi State</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>NC State</t>
+          <t>Texas</t>
         </is>
       </c>
       <c r="D21" t="n">
-        <v>8.4</v>
+        <v>8.699999999999999</v>
       </c>
       <c r="E21" t="n">
-        <v>2.9</v>
+        <v>3.1</v>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>Pittsburgh -8.5</t>
+          <t>Texas -6.5</t>
         </is>
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>Pittsburgh -7.0</t>
+          <t>Texas -6.5</t>
         </is>
       </c>
       <c r="H21" t="inlineStr">
         <is>
-          <t>Pittsburgh -9.9</t>
+          <t>Texas -9.6</t>
         </is>
       </c>
       <c r="I21" t="n">
-        <v>9.9</v>
+        <v>-9.6</v>
       </c>
       <c r="J21" t="n">
-        <v>7</v>
+        <v>-6.5</v>
       </c>
       <c r="K21" t="inlineStr"/>
       <c r="L21" t="inlineStr"/>
@@ -1516,40 +1516,40 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Tulsa</t>
+          <t>Wake Forest</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>Temple</t>
+          <t>SMU</t>
         </is>
       </c>
       <c r="D22" t="n">
-        <v>4.3</v>
+        <v>7.8</v>
       </c>
       <c r="E22" t="n">
-        <v>2.699999999999999</v>
+        <v>3</v>
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>Temple -6.0</t>
+          <t>SMU -3.5</t>
         </is>
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>Temple -6.0</t>
+          <t>SMU -3.5</t>
         </is>
       </c>
       <c r="H22" t="inlineStr">
         <is>
-          <t>Temple -8.7</t>
+          <t>SMU -6.5</t>
         </is>
       </c>
       <c r="I22" t="n">
-        <v>-8.699999999999999</v>
+        <v>-6.5</v>
       </c>
       <c r="J22" t="n">
-        <v>-6</v>
+        <v>-3.5</v>
       </c>
       <c r="K22" t="inlineStr"/>
       <c r="L22" t="inlineStr"/>
@@ -1616,40 +1616,40 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>Cincinnati</t>
+          <t>Texas Tech</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>Baylor</t>
+          <t>Oklahoma State</t>
         </is>
       </c>
       <c r="D24" t="n">
-        <v>8.9</v>
+        <v>3.1</v>
       </c>
       <c r="E24" t="n">
-        <v>2.4</v>
+        <v>2.299999999999997</v>
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>Cincinnati -5.5</t>
+          <t>Texas Tech -39.0</t>
         </is>
       </c>
       <c r="G24" t="inlineStr">
         <is>
-          <t>Cincinnati -5.5</t>
+          <t>Texas Tech -38.5</t>
         </is>
       </c>
       <c r="H24" t="inlineStr">
         <is>
-          <t>Cincinnati -7.9</t>
+          <t>Texas Tech -40.8</t>
         </is>
       </c>
       <c r="I24" t="n">
-        <v>7.9</v>
+        <v>40.8</v>
       </c>
       <c r="J24" t="n">
-        <v>5.5</v>
+        <v>38.5</v>
       </c>
       <c r="K24" t="inlineStr"/>
       <c r="L24" t="inlineStr"/>
@@ -1666,40 +1666,40 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>Texas Tech</t>
+          <t>Navy</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>Oklahoma State</t>
+          <t>Florida Atlantic</t>
         </is>
       </c>
       <c r="D25" t="n">
-        <v>3.1</v>
+        <v>4.5</v>
       </c>
       <c r="E25" t="n">
-        <v>2.299999999999997</v>
+        <v>2.199999999999999</v>
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>Texas Tech -39.0</t>
+          <t>Navy -14.0</t>
         </is>
       </c>
       <c r="G25" t="inlineStr">
         <is>
-          <t>Texas Tech -38.5</t>
+          <t>Navy -15.0</t>
         </is>
       </c>
       <c r="H25" t="inlineStr">
         <is>
-          <t>Texas Tech -40.8</t>
+          <t>Navy -17.2</t>
         </is>
       </c>
       <c r="I25" t="n">
-        <v>40.8</v>
+        <v>17.2</v>
       </c>
       <c r="J25" t="n">
-        <v>38.5</v>
+        <v>15</v>
       </c>
       <c r="K25" t="inlineStr"/>
       <c r="L25" t="inlineStr"/>
@@ -1716,40 +1716,40 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>Navy</t>
+          <t>Tulsa</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>Florida Atlantic</t>
+          <t>Temple</t>
         </is>
       </c>
       <c r="D26" t="n">
-        <v>4.5</v>
+        <v>4.3</v>
       </c>
       <c r="E26" t="n">
         <v>2.199999999999999</v>
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>Navy -14.0</t>
+          <t>Temple -6.0</t>
         </is>
       </c>
       <c r="G26" t="inlineStr">
         <is>
-          <t>Navy -15.0</t>
+          <t>Temple -6.5</t>
         </is>
       </c>
       <c r="H26" t="inlineStr">
         <is>
-          <t>Navy -17.2</t>
+          <t>Temple -8.7</t>
         </is>
       </c>
       <c r="I26" t="n">
-        <v>17.2</v>
+        <v>-8.699999999999999</v>
       </c>
       <c r="J26" t="n">
-        <v>15</v>
+        <v>-6.5</v>
       </c>
       <c r="K26" t="inlineStr"/>
       <c r="L26" t="inlineStr"/>
@@ -2166,40 +2166,40 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>Kent State</t>
+          <t>Arkansas State</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>Bowling Green</t>
+          <t>Georgia Southern</t>
         </is>
       </c>
       <c r="D35" t="n">
-        <v>2.8</v>
+        <v>5.8</v>
       </c>
       <c r="E35" t="n">
-        <v>1.300000000000001</v>
+        <v>1.4</v>
       </c>
       <c r="F35" t="inlineStr">
         <is>
-          <t>Bowling Green -8.5</t>
+          <t>Arkansas State -2.0</t>
         </is>
       </c>
       <c r="G35" t="inlineStr">
         <is>
-          <t>Bowling Green -8.5</t>
+          <t>Arkansas State -2.5</t>
         </is>
       </c>
       <c r="H35" t="inlineStr">
         <is>
-          <t>Bowling Green -9.8</t>
+          <t>Arkansas State -1.1</t>
         </is>
       </c>
       <c r="I35" t="n">
-        <v>-9.800000000000001</v>
+        <v>1.1</v>
       </c>
       <c r="J35" t="n">
-        <v>-8.5</v>
+        <v>2.5</v>
       </c>
       <c r="K35" t="inlineStr"/>
       <c r="L35" t="inlineStr"/>
@@ -2216,40 +2216,40 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>Vanderbilt</t>
+          <t>South Carolina</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>Missouri</t>
+          <t>Alabama</t>
         </is>
       </c>
       <c r="D36" t="n">
-        <v>9.699999999999999</v>
+        <v>8.4</v>
       </c>
       <c r="E36" t="n">
-        <v>1.2</v>
+        <v>1.300000000000001</v>
       </c>
       <c r="F36" t="inlineStr">
         <is>
-          <t>Vanderbilt -3.0</t>
+          <t>Alabama -13.0</t>
         </is>
       </c>
       <c r="G36" t="inlineStr">
         <is>
-          <t>Vanderbilt -3.0</t>
+          <t>Alabama -11.5</t>
         </is>
       </c>
       <c r="H36" t="inlineStr">
         <is>
-          <t>Vanderbilt -1.8</t>
+          <t>Alabama -12.8</t>
         </is>
       </c>
       <c r="I36" t="n">
-        <v>1.8</v>
+        <v>-12.8</v>
       </c>
       <c r="J36" t="n">
-        <v>3</v>
+        <v>-11.5</v>
       </c>
       <c r="K36" t="inlineStr"/>
       <c r="L36" t="inlineStr"/>
@@ -2266,40 +2266,40 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>Charlotte</t>
+          <t>Kent State</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>North Texas</t>
+          <t>Bowling Green</t>
         </is>
       </c>
       <c r="D37" t="n">
-        <v>1.9</v>
+        <v>2.8</v>
       </c>
       <c r="E37" t="n">
-        <v>1.100000000000001</v>
+        <v>1.300000000000001</v>
       </c>
       <c r="F37" t="inlineStr">
         <is>
-          <t>North Texas -27.0</t>
+          <t>Bowling Green -8.5</t>
         </is>
       </c>
       <c r="G37" t="inlineStr">
         <is>
-          <t>North Texas -27.0</t>
+          <t>Bowling Green -8.5</t>
         </is>
       </c>
       <c r="H37" t="inlineStr">
         <is>
-          <t>North Texas -28.1</t>
+          <t>Bowling Green -9.8</t>
         </is>
       </c>
       <c r="I37" t="n">
-        <v>-28.1</v>
+        <v>-9.800000000000001</v>
       </c>
       <c r="J37" t="n">
-        <v>-27</v>
+        <v>-8.5</v>
       </c>
       <c r="K37" t="inlineStr"/>
       <c r="L37" t="inlineStr"/>
@@ -2316,40 +2316,40 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>Arkansas</t>
+          <t>Vanderbilt</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>Auburn</t>
+          <t>Missouri</t>
         </is>
       </c>
       <c r="D38" t="n">
-        <v>9.199999999999999</v>
+        <v>9.699999999999999</v>
       </c>
       <c r="E38" t="n">
-        <v>1.1</v>
+        <v>1.2</v>
       </c>
       <c r="F38" t="inlineStr">
         <is>
-          <t>Arkansas --0.0</t>
+          <t>Vanderbilt -3.0</t>
         </is>
       </c>
       <c r="G38" t="inlineStr">
         <is>
-          <t>Auburn -1.5</t>
+          <t>Vanderbilt -3.0</t>
         </is>
       </c>
       <c r="H38" t="inlineStr">
         <is>
-          <t>Auburn -0.4</t>
+          <t>Vanderbilt -1.8</t>
         </is>
       </c>
       <c r="I38" t="n">
-        <v>-0.4</v>
+        <v>1.8</v>
       </c>
       <c r="J38" t="n">
-        <v>-1.5</v>
+        <v>3</v>
       </c>
       <c r="K38" t="inlineStr"/>
       <c r="L38" t="inlineStr"/>
@@ -2366,40 +2366,40 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>West Virginia</t>
+          <t>Charlotte</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>TCU</t>
+          <t>North Texas</t>
         </is>
       </c>
       <c r="D39" t="n">
-        <v>5.8</v>
+        <v>1.9</v>
       </c>
       <c r="E39" t="n">
-        <v>0.9000000000000004</v>
+        <v>1.100000000000001</v>
       </c>
       <c r="F39" t="inlineStr">
         <is>
-          <t>TCU -15.0</t>
+          <t>North Texas -27.0</t>
         </is>
       </c>
       <c r="G39" t="inlineStr">
         <is>
-          <t>TCU -15.0</t>
+          <t>North Texas -27.0</t>
         </is>
       </c>
       <c r="H39" t="inlineStr">
         <is>
-          <t>TCU -14.1</t>
+          <t>North Texas -28.1</t>
         </is>
       </c>
       <c r="I39" t="n">
-        <v>-14.1</v>
+        <v>-28.1</v>
       </c>
       <c r="J39" t="n">
-        <v>-15</v>
+        <v>-27</v>
       </c>
       <c r="K39" t="inlineStr"/>
       <c r="L39" t="inlineStr"/>
@@ -2416,40 +2416,40 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>Washington</t>
+          <t>Arkansas</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>Illinois</t>
+          <t>Auburn</t>
         </is>
       </c>
       <c r="D40" t="n">
-        <v>9.5</v>
+        <v>9.199999999999999</v>
       </c>
       <c r="E40" t="n">
-        <v>0.8999999999999999</v>
+        <v>1.1</v>
       </c>
       <c r="F40" t="inlineStr">
         <is>
-          <t>Washington -5.0</t>
+          <t>Arkansas --0.0</t>
         </is>
       </c>
       <c r="G40" t="inlineStr">
         <is>
-          <t>Washington -4.5</t>
+          <t>Auburn -1.5</t>
         </is>
       </c>
       <c r="H40" t="inlineStr">
         <is>
-          <t>Washington -3.6</t>
+          <t>Auburn -0.4</t>
         </is>
       </c>
       <c r="I40" t="n">
-        <v>3.6</v>
+        <v>-0.4</v>
       </c>
       <c r="J40" t="n">
-        <v>4.5</v>
+        <v>-1.5</v>
       </c>
       <c r="K40" t="inlineStr"/>
       <c r="L40" t="inlineStr"/>
@@ -2466,40 +2466,40 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>Arkansas State</t>
+          <t>Virginia Tech</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>Georgia Southern</t>
+          <t>California</t>
         </is>
       </c>
       <c r="D41" t="n">
-        <v>5.8</v>
+        <v>7.8</v>
       </c>
       <c r="E41" t="n">
-        <v>0.8999999999999999</v>
+        <v>1</v>
       </c>
       <c r="F41" t="inlineStr">
         <is>
-          <t>Arkansas State -2.0</t>
+          <t>Virginia Tech -4.5</t>
         </is>
       </c>
       <c r="G41" t="inlineStr">
         <is>
-          <t>Arkansas State -2.0</t>
+          <t>Virginia Tech -4.5</t>
         </is>
       </c>
       <c r="H41" t="inlineStr">
         <is>
-          <t>Arkansas State -1.1</t>
+          <t>Virginia Tech -3.5</t>
         </is>
       </c>
       <c r="I41" t="n">
-        <v>1.1</v>
+        <v>3.5</v>
       </c>
       <c r="J41" t="n">
-        <v>2</v>
+        <v>4.5</v>
       </c>
       <c r="K41" t="inlineStr"/>
       <c r="L41" t="inlineStr"/>
@@ -2516,40 +2516,40 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>Purdue</t>
+          <t>West Virginia</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>Rutgers</t>
+          <t>TCU</t>
         </is>
       </c>
       <c r="D42" t="n">
-        <v>7.7</v>
+        <v>5.8</v>
       </c>
       <c r="E42" t="n">
-        <v>0.8</v>
+        <v>0.9000000000000004</v>
       </c>
       <c r="F42" t="inlineStr">
         <is>
-          <t>Rutgers -2.5</t>
+          <t>TCU -15.0</t>
         </is>
       </c>
       <c r="G42" t="inlineStr">
         <is>
-          <t>Rutgers -2.5</t>
+          <t>TCU -15.0</t>
         </is>
       </c>
       <c r="H42" t="inlineStr">
         <is>
-          <t>Rutgers -1.7</t>
+          <t>TCU -14.1</t>
         </is>
       </c>
       <c r="I42" t="n">
-        <v>-1.7</v>
+        <v>-14.1</v>
       </c>
       <c r="J42" t="n">
-        <v>-2.5</v>
+        <v>-15</v>
       </c>
       <c r="K42" t="inlineStr"/>
       <c r="L42" t="inlineStr"/>
@@ -2566,40 +2566,40 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>Florida International</t>
+          <t>Washington</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>Kennesaw State</t>
+          <t>Illinois</t>
         </is>
       </c>
       <c r="D43" t="n">
-        <v>4.8</v>
+        <v>9.5</v>
       </c>
       <c r="E43" t="n">
-        <v>0.7000000000000002</v>
+        <v>0.8999999999999999</v>
       </c>
       <c r="F43" t="inlineStr">
         <is>
-          <t>Kennesaw State -1.5</t>
+          <t>Washington -5.0</t>
         </is>
       </c>
       <c r="G43" t="inlineStr">
         <is>
-          <t>Kennesaw State -3.0</t>
+          <t>Washington -4.5</t>
         </is>
       </c>
       <c r="H43" t="inlineStr">
         <is>
-          <t>Kennesaw State -3.7</t>
+          <t>Washington -3.6</t>
         </is>
       </c>
       <c r="I43" t="n">
-        <v>-3.7</v>
+        <v>3.6</v>
       </c>
       <c r="J43" t="n">
-        <v>-3</v>
+        <v>4.5</v>
       </c>
       <c r="K43" t="inlineStr"/>
       <c r="L43" t="inlineStr"/>
@@ -2616,40 +2616,40 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>Georgia State</t>
+          <t>Purdue</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>South Alabama</t>
+          <t>Rutgers</t>
         </is>
       </c>
       <c r="D44" t="n">
-        <v>3.5</v>
+        <v>7.7</v>
       </c>
       <c r="E44" t="n">
-        <v>0.7000000000000002</v>
+        <v>0.8</v>
       </c>
       <c r="F44" t="inlineStr">
         <is>
-          <t>South Alabama -6.0</t>
+          <t>Rutgers -2.5</t>
         </is>
       </c>
       <c r="G44" t="inlineStr">
         <is>
-          <t>South Alabama -6.5</t>
+          <t>Rutgers -2.5</t>
         </is>
       </c>
       <c r="H44" t="inlineStr">
         <is>
-          <t>South Alabama -7.2</t>
+          <t>Rutgers -1.7</t>
         </is>
       </c>
       <c r="I44" t="n">
-        <v>-7.2</v>
+        <v>-1.7</v>
       </c>
       <c r="J44" t="n">
-        <v>-6.5</v>
+        <v>-2.5</v>
       </c>
       <c r="K44" t="inlineStr"/>
       <c r="L44" t="inlineStr"/>
@@ -2666,40 +2666,40 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>Louisville</t>
+          <t>Florida International</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>Boston College</t>
+          <t>Kennesaw State</t>
         </is>
       </c>
       <c r="D45" t="n">
-        <v>4.6</v>
+        <v>4.8</v>
       </c>
       <c r="E45" t="n">
-        <v>0.6000000000000014</v>
+        <v>0.7000000000000002</v>
       </c>
       <c r="F45" t="inlineStr">
         <is>
-          <t>Louisville -24.5</t>
+          <t>Kennesaw State -1.5</t>
         </is>
       </c>
       <c r="G45" t="inlineStr">
         <is>
-          <t>Louisville -25.0</t>
+          <t>Kennesaw State -3.0</t>
         </is>
       </c>
       <c r="H45" t="inlineStr">
         <is>
-          <t>Louisville -25.6</t>
+          <t>Kennesaw State -3.7</t>
         </is>
       </c>
       <c r="I45" t="n">
-        <v>25.6</v>
+        <v>-3.7</v>
       </c>
       <c r="J45" t="n">
-        <v>25</v>
+        <v>-3</v>
       </c>
       <c r="K45" t="inlineStr"/>
       <c r="L45" t="inlineStr"/>
@@ -2716,40 +2716,40 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>Miami</t>
+          <t>Georgia State</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>Stanford</t>
+          <t>South Alabama</t>
         </is>
       </c>
       <c r="D46" t="n">
-        <v>4.5</v>
+        <v>3.5</v>
       </c>
       <c r="E46" t="n">
-        <v>0.5</v>
+        <v>0.7000000000000002</v>
       </c>
       <c r="F46" t="inlineStr">
         <is>
-          <t>Miami -30.0</t>
+          <t>South Alabama -6.0</t>
         </is>
       </c>
       <c r="G46" t="inlineStr">
         <is>
-          <t>Miami -30.0</t>
+          <t>South Alabama -6.5</t>
         </is>
       </c>
       <c r="H46" t="inlineStr">
         <is>
-          <t>Miami -30.5</t>
+          <t>South Alabama -7.2</t>
         </is>
       </c>
       <c r="I46" t="n">
-        <v>30.5</v>
+        <v>-7.2</v>
       </c>
       <c r="J46" t="n">
-        <v>30</v>
+        <v>-6.5</v>
       </c>
       <c r="K46" t="inlineStr"/>
       <c r="L46" t="inlineStr"/>
@@ -2766,40 +2766,40 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>Georgia Tech</t>
+          <t>Louisville</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>Syracuse</t>
+          <t>Boston College</t>
         </is>
       </c>
       <c r="D47" t="n">
-        <v>6.9</v>
+        <v>4.6</v>
       </c>
       <c r="E47" t="n">
-        <v>0.5</v>
+        <v>0.6000000000000014</v>
       </c>
       <c r="F47" t="inlineStr">
         <is>
-          <t>Georgia Tech -18.0</t>
+          <t>Louisville -24.5</t>
         </is>
       </c>
       <c r="G47" t="inlineStr">
         <is>
-          <t>Georgia Tech -17.5</t>
+          <t>Louisville -25.0</t>
         </is>
       </c>
       <c r="H47" t="inlineStr">
         <is>
-          <t>Georgia Tech -17.0</t>
+          <t>Louisville -25.6</t>
         </is>
       </c>
       <c r="I47" t="n">
-        <v>17</v>
+        <v>25.6</v>
       </c>
       <c r="J47" t="n">
-        <v>17.5</v>
+        <v>25</v>
       </c>
       <c r="K47" t="inlineStr"/>
       <c r="L47" t="inlineStr"/>
@@ -2816,40 +2816,40 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>Virginia Tech</t>
+          <t>Miami</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>California</t>
+          <t>Stanford</t>
         </is>
       </c>
       <c r="D48" t="n">
-        <v>7.8</v>
+        <v>4.5</v>
       </c>
       <c r="E48" t="n">
         <v>0.5</v>
       </c>
       <c r="F48" t="inlineStr">
         <is>
-          <t>Virginia Tech -4.5</t>
+          <t>Miami -30.0</t>
         </is>
       </c>
       <c r="G48" t="inlineStr">
         <is>
-          <t>Virginia Tech -4.0</t>
+          <t>Miami -30.0</t>
         </is>
       </c>
       <c r="H48" t="inlineStr">
         <is>
-          <t>Virginia Tech -3.5</t>
+          <t>Miami -30.5</t>
         </is>
       </c>
       <c r="I48" t="n">
-        <v>3.5</v>
+        <v>30.5</v>
       </c>
       <c r="J48" t="n">
-        <v>4</v>
+        <v>30</v>
       </c>
       <c r="K48" t="inlineStr"/>
       <c r="L48" t="inlineStr"/>
@@ -2866,40 +2866,40 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>Kentucky</t>
+          <t>Georgia Tech</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>Tennessee</t>
+          <t>Syracuse</t>
         </is>
       </c>
       <c r="D49" t="n">
-        <v>8.199999999999999</v>
+        <v>6.9</v>
       </c>
       <c r="E49" t="n">
-        <v>0.4000000000000004</v>
+        <v>0.5</v>
       </c>
       <c r="F49" t="inlineStr">
         <is>
-          <t>Tennessee -9.0</t>
+          <t>Georgia Tech -18.0</t>
         </is>
       </c>
       <c r="G49" t="inlineStr">
         <is>
-          <t>Tennessee -9.5</t>
+          <t>Georgia Tech -17.5</t>
         </is>
       </c>
       <c r="H49" t="inlineStr">
         <is>
-          <t>Tennessee -9.1</t>
+          <t>Georgia Tech -17.0</t>
         </is>
       </c>
       <c r="I49" t="n">
-        <v>-9.1</v>
+        <v>17</v>
       </c>
       <c r="J49" t="n">
-        <v>-9.5</v>
+        <v>17.5</v>
       </c>
       <c r="K49" t="inlineStr"/>
       <c r="L49" t="inlineStr"/>
@@ -2916,40 +2916,40 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>New Mexico</t>
+          <t>Kentucky</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>Utah State</t>
+          <t>Tennessee</t>
         </is>
       </c>
       <c r="D50" t="n">
-        <v>7.5</v>
+        <v>8.199999999999999</v>
       </c>
       <c r="E50" t="n">
-        <v>0.3999999999999999</v>
+        <v>0.4000000000000004</v>
       </c>
       <c r="F50" t="inlineStr">
         <is>
-          <t>New Mexico -2.5</t>
+          <t>Tennessee -9.0</t>
         </is>
       </c>
       <c r="G50" t="inlineStr">
         <is>
-          <t>New Mexico -2.5</t>
+          <t>Tennessee -9.5</t>
         </is>
       </c>
       <c r="H50" t="inlineStr">
         <is>
-          <t>New Mexico -2.9</t>
+          <t>Tennessee -9.1</t>
         </is>
       </c>
       <c r="I50" t="n">
-        <v>2.9</v>
+        <v>-9.1</v>
       </c>
       <c r="J50" t="n">
-        <v>2.5</v>
+        <v>-9.5</v>
       </c>
       <c r="K50" t="inlineStr"/>
       <c r="L50" t="inlineStr"/>
@@ -2966,40 +2966,40 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>Oklahoma</t>
+          <t>New Mexico</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>Ole Miss</t>
+          <t>Utah State</t>
         </is>
       </c>
       <c r="D51" t="n">
-        <v>9.699999999999999</v>
+        <v>7.5</v>
       </c>
       <c r="E51" t="n">
-        <v>0.2999999999999998</v>
+        <v>0.3999999999999999</v>
       </c>
       <c r="F51" t="inlineStr">
         <is>
-          <t>Oklahoma -4.5</t>
+          <t>New Mexico -2.5</t>
         </is>
       </c>
       <c r="G51" t="inlineStr">
         <is>
-          <t>Oklahoma -4.0</t>
+          <t>New Mexico -2.5</t>
         </is>
       </c>
       <c r="H51" t="inlineStr">
         <is>
-          <t>Oklahoma -4.3</t>
+          <t>New Mexico -2.9</t>
         </is>
       </c>
       <c r="I51" t="n">
-        <v>4.3</v>
+        <v>2.9</v>
       </c>
       <c r="J51" t="n">
-        <v>4</v>
+        <v>2.5</v>
       </c>
       <c r="K51" t="inlineStr"/>
       <c r="L51" t="inlineStr"/>
@@ -3016,40 +3016,40 @@
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>Fresno State</t>
+          <t>Oklahoma</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>San Diego State</t>
+          <t>Ole Miss</t>
         </is>
       </c>
       <c r="D52" t="n">
-        <v>6.9</v>
+        <v>9.699999999999999</v>
       </c>
       <c r="E52" t="n">
-        <v>0.2000000000000002</v>
+        <v>0.2999999999999998</v>
       </c>
       <c r="F52" t="inlineStr">
         <is>
-          <t>San Diego State -2.5</t>
+          <t>Oklahoma -4.5</t>
         </is>
       </c>
       <c r="G52" t="inlineStr">
         <is>
-          <t>San Diego State -3.5</t>
+          <t>Oklahoma -4.0</t>
         </is>
       </c>
       <c r="H52" t="inlineStr">
         <is>
-          <t>San Diego State -3.7</t>
+          <t>Oklahoma -4.3</t>
         </is>
       </c>
       <c r="I52" t="n">
-        <v>-3.7</v>
+        <v>4.3</v>
       </c>
       <c r="J52" t="n">
-        <v>-3.5</v>
+        <v>4</v>
       </c>
       <c r="K52" t="inlineStr"/>
       <c r="L52" t="inlineStr"/>
@@ -3066,40 +3066,40 @@
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>South Carolina</t>
+          <t>Fresno State</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>Alabama</t>
+          <t>San Diego State</t>
         </is>
       </c>
       <c r="D53" t="n">
-        <v>8.4</v>
+        <v>6.9</v>
       </c>
       <c r="E53" t="n">
-        <v>0.1999999999999993</v>
+        <v>0.2000000000000002</v>
       </c>
       <c r="F53" t="inlineStr">
         <is>
-          <t>Alabama -13.0</t>
+          <t>San Diego State -2.5</t>
         </is>
       </c>
       <c r="G53" t="inlineStr">
         <is>
-          <t>Alabama -13.0</t>
+          <t>San Diego State -3.5</t>
         </is>
       </c>
       <c r="H53" t="inlineStr">
         <is>
-          <t>Alabama -12.8</t>
+          <t>San Diego State -3.7</t>
         </is>
       </c>
       <c r="I53" t="n">
-        <v>-12.8</v>
+        <v>-3.7</v>
       </c>
       <c r="J53" t="n">
-        <v>-13</v>
+        <v>-3.5</v>
       </c>
       <c r="K53" t="inlineStr"/>
       <c r="L53" t="inlineStr"/>

</xml_diff>